<commit_message>
Added script event handler
</commit_message>
<xml_diff>
--- a/npc/npc.xlsx
+++ b/npc/npc.xlsx
@@ -91,7 +91,7 @@
     <t xml:space="preserve">No problem!</t>
   </si>
   <si>
-    <t xml:space="preserve">scriptevent game1:npcComplete 0</t>
+    <t xml:space="preserve">scriptevent rod:npcComplete 0</t>
   </si>
   <si>
     <t xml:space="preserve">rodNpc0Fail</t>
@@ -103,7 +103,7 @@
     <t xml:space="preserve">Show me </t>
   </si>
   <si>
-    <t xml:space="preserve">scriptevent game1:npcReplay 0</t>
+    <t xml:space="preserve">scriptevent rod:npcReplay 0</t>
   </si>
   <si>
     <t xml:space="preserve">Not Interested!</t>
@@ -124,7 +124,7 @@
     <t xml:space="preserve">You’re Welcome</t>
   </si>
   <si>
-    <t xml:space="preserve">scriptevent game1:npcComplete 1</t>
+    <t xml:space="preserve">scriptevent rod:npcComplete 1</t>
   </si>
   <si>
     <t xml:space="preserve">rodNpc1Fail</t>
@@ -133,7 +133,7 @@
     <t xml:space="preserve">Well done you made it! Shall I show you a more optimum route? </t>
   </si>
   <si>
-    <t xml:space="preserve">scriptevent game1:npcReplay 1</t>
+    <t xml:space="preserve">scriptevent rod:npcReplay 1</t>
   </si>
 </sst>
 </file>
@@ -344,10 +344,10 @@
   <dimension ref="A1:R77"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="109" zoomScaleNormal="109" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.41"/>

</xml_diff>

<commit_message>
The game flows nicely!
</commit_message>
<xml_diff>
--- a/npc/npc.xlsx
+++ b/npc/npc.xlsx
@@ -307,7 +307,7 @@
     <t xml:space="preserve">npc8</t>
   </si>
   <si>
-    <t xml:space="preserve">Great work you simplified 3/8 to 1/8 and ¼.</t>
+    <t xml:space="preserve">Great work you simplified 2/8 to 1/4.</t>
   </si>
   <si>
     <t xml:space="preserve">scriptevent rod:npcComplete 9</t>
@@ -736,7 +736,7 @@
   <dimension ref="A1:R87"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="109" zoomScaleNormal="109" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B44" activeCellId="0" sqref="B44"/>
+      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Started npc index from 0
</commit_message>
<xml_diff>
--- a/npc/npc.xlsx
+++ b/npc/npc.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="134">
   <si>
     <t xml:space="preserve">Scene</t>
   </si>
@@ -91,301 +91,307 @@
     <t xml:space="preserve">No problem!</t>
   </si>
   <si>
+    <t xml:space="preserve">scriptevent rod:npcComplete 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc0Fail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You saved me! You made up a half out of multiple fractions. I can show you a more optimum way. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show me </t>
+  </si>
+  <si>
+    <t xml:space="preserve">scriptevent rod:npcReplay 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not Interested!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc0Default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEEEEELLLLPPPPPPP!!!!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coming!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc1Win</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">npc1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Woohoo, 6 is a quarter of 24.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You’re Welcome</t>
+  </si>
+  <si>
     <t xml:space="preserve">scriptevent rod:npcComplete 1</t>
   </si>
   <si>
-    <t xml:space="preserve">rodNpc0Fail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You saved me! You made up a half out of multiple fractions. I can show you a more optimum way. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Show me </t>
+    <t xml:space="preserve">rodNpc1Fail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Well done you made it! Shall I show you a more optimum route? </t>
   </si>
   <si>
     <t xml:space="preserve">scriptevent rod:npcReplay 1</t>
   </si>
   <si>
-    <t xml:space="preserve">Not Interested!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc0Default</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEEEEELLLLPPPPPPP!!!!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coming!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc1Win</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">npc1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Woohoo, 6 is a quarter of 24.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You’re Welcome</t>
+    <t xml:space="preserve">rodNpc1Default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc2Win</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">npc2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 is a third of 24.</t>
   </si>
   <si>
     <t xml:space="preserve">scriptevent rod:npcComplete 2</t>
   </si>
   <si>
-    <t xml:space="preserve">rodNpc1Fail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Well done you made it! Shall I show you a more optimum route? </t>
+    <t xml:space="preserve">rodNpc2Fail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You saved me! Shall I show you a more optimum route?</t>
   </si>
   <si>
     <t xml:space="preserve">scriptevent rod:npcReplay 2</t>
   </si>
   <si>
-    <t xml:space="preserve">rodNpc1Default</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc2Win</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">npc2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8 is a third of 24.</t>
+    <t xml:space="preserve">rodNpc2Default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc3Win</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">npc3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 is a sixth of 24.</t>
   </si>
   <si>
     <t xml:space="preserve">scriptevent rod:npcComplete 3</t>
   </si>
   <si>
-    <t xml:space="preserve">rodNpc2Fail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You saved me! Shall I show you a more optimum route?</t>
+    <t xml:space="preserve">rodNpc3Fail</t>
   </si>
   <si>
     <t xml:space="preserve">scriptevent rod:npcReplay 3</t>
   </si>
   <si>
-    <t xml:space="preserve">rodNpc2Default</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc3Win</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">npc3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 is a sixth of 24.</t>
+    <t xml:space="preserve">rodNpc3Default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc4Win</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">npc4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Well done you simplified 2/6 to 1/3!  </t>
   </si>
   <si>
     <t xml:space="preserve">scriptevent rod:npcComplete 4</t>
   </si>
   <si>
-    <t xml:space="preserve">rodNpc3Fail</t>
+    <t xml:space="preserve">rodNpc4Fail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You saved me but if you simplify the fraction you could have got here in less rods! Shall I show you?</t>
   </si>
   <si>
     <t xml:space="preserve">scriptevent rod:npcReplay 4</t>
   </si>
   <si>
-    <t xml:space="preserve">rodNpc3Default</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc4Win</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">npc4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Well done you simplified 2/6 to 1/3!  </t>
+    <t xml:space="preserve">rodNpc4Default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc5Win</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">npc5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skipped</t>
   </si>
   <si>
     <t xml:space="preserve">scriptevent rod:npcComplete 5</t>
   </si>
   <si>
-    <t xml:space="preserve">rodNpc4Fail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You saved me but if you simplify the fraction you could have got here in less rods! Shall I show you?</t>
+    <t xml:space="preserve">rodNpc5Fail</t>
   </si>
   <si>
     <t xml:space="preserve">scriptevent rod:npcReplay 5</t>
   </si>
   <si>
-    <t xml:space="preserve">rodNpc4Default</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc5Win</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">npc5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Skipped</t>
+    <t xml:space="preserve">rodNpc5Default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc6Win</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">npc6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yep 2/1 is 48 great work.</t>
   </si>
   <si>
     <t xml:space="preserve">scriptevent rod:npcComplete 6</t>
   </si>
   <si>
-    <t xml:space="preserve">rodNpc5Fail</t>
+    <t xml:space="preserve">rodNpc6Fail</t>
   </si>
   <si>
     <t xml:space="preserve">scriptevent rod:npcReplay 6</t>
   </si>
   <si>
-    <t xml:space="preserve">rodNpc5Default</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc6Win</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">npc6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yep 2/1 is 48 great work.</t>
+    <t xml:space="preserve">rodNpc6Default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc7Win</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">npc7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Three is indeed 1/8 of 24.</t>
   </si>
   <si>
     <t xml:space="preserve">scriptevent rod:npcComplete 7</t>
   </si>
   <si>
-    <t xml:space="preserve">rodNpc6Fail</t>
+    <t xml:space="preserve">rodNpc7Fail</t>
   </si>
   <si>
     <t xml:space="preserve">scriptevent rod:npcReplay 7</t>
   </si>
   <si>
-    <t xml:space="preserve">rodNpc6Default</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc7Win</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">npc7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Three is indeed 1/8 of 24.</t>
+    <t xml:space="preserve">rodNpc7Default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc8Win</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">npc8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Great work you simplified 2/8 to 1/4.</t>
   </si>
   <si>
     <t xml:space="preserve">scriptevent rod:npcComplete 8</t>
   </si>
   <si>
-    <t xml:space="preserve">rodNpc7Fail</t>
+    <t xml:space="preserve">rodNpc8Fail</t>
   </si>
   <si>
     <t xml:space="preserve">scriptevent rod:npcReplay 8</t>
   </si>
   <si>
-    <t xml:space="preserve">rodNpc7Default</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc8Win</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">npc8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Great work you simplified 2/8 to 1/4.</t>
+    <t xml:space="preserve">rodNpc8Default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc9Win</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">npc9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Two is 1/12 of24</t>
   </si>
   <si>
     <t xml:space="preserve">scriptevent rod:npcComplete 9</t>
   </si>
   <si>
-    <t xml:space="preserve">rodNpc8Fail</t>
+    <t xml:space="preserve">rodNpc9Fail</t>
   </si>
   <si>
     <t xml:space="preserve">scriptevent rod:npcReplay 9</t>
   </si>
   <si>
-    <t xml:space="preserve">rodNpc8Default</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc9Win</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">npc9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Two is 1/12 of24</t>
+    <t xml:space="preserve">rodNpc9Default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc10Win</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">npc10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Great work simplifying the fraction from 2/12 to 1/6.</t>
   </si>
   <si>
     <t xml:space="preserve">scriptevent rod:npcComplete 10</t>
   </si>
   <si>
-    <t xml:space="preserve">rodNpc9Fail</t>
+    <t xml:space="preserve">rodNpc10Fail</t>
   </si>
   <si>
     <t xml:space="preserve">scriptevent rod:npcReplay 10</t>
   </si>
   <si>
-    <t xml:space="preserve">rodNpc9Default</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc10Win</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">npc10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Great work simplifying the fraction from 2/12 to 1/6.</t>
+    <t xml:space="preserve">rodNpc10Default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc11Win</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">npc11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You’ve done very well to get to me! I thought I was never going to be saved.</t>
   </si>
   <si>
     <t xml:space="preserve">scriptevent rod:npcComplete 11</t>
   </si>
   <si>
-    <t xml:space="preserve">rodNpc10Fail</t>
+    <t xml:space="preserve">rodNpc11Fail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I won’t ever say this, if you see this something has gone wrong!</t>
   </si>
   <si>
     <t xml:space="preserve">scriptevent rod:npcReplay 11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc10Default</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc11Win</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">npc11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You’ve done very well to get to me! I thought I was never going to be saved.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc11Fail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I won’t ever say this, if you see this something has gone wrong!</t>
   </si>
   <si>
     <t xml:space="preserve">rodNpc11Default</t>
@@ -735,8 +741,8 @@
   </sheetPr>
   <dimension ref="A1:R87"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="109" zoomScaleNormal="109" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G7" colorId="64" zoomScale="109" zoomScaleNormal="109" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H42" activeCellId="0" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1505,12 +1511,12 @@
         <v>36</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>117</v>
@@ -1519,13 +1525,13 @@
         <v>118</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>26</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="I36" s="1" t="s">
         <v>28</v>
@@ -1533,7 +1539,7 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>117</v>
@@ -1551,42 +1557,42 @@
     </row>
     <row r="38" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>26</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>28</v>
@@ -1594,13 +1600,13 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
Npcs go home and  wandering traders are no more
</commit_message>
<xml_diff>
--- a/npc/npc.xlsx
+++ b/npc/npc.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="141">
   <si>
     <t xml:space="preserve">Scene</t>
   </si>
@@ -118,6 +118,12 @@
     <t xml:space="preserve">Coming!</t>
   </si>
   <si>
+    <t xml:space="preserve">rodNpc0Saved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Few I’m back all thanks to you.</t>
+  </si>
+  <si>
     <t xml:space="preserve">rodNpc1Win</t>
   </si>
   <si>
@@ -148,6 +154,9 @@
     <t xml:space="preserve">rodNpc1Default</t>
   </si>
   <si>
+    <t xml:space="preserve">rodNpc1Saved</t>
+  </si>
+  <si>
     <t xml:space="preserve">rodNpc2Win</t>
   </si>
   <si>
@@ -175,6 +184,9 @@
     <t xml:space="preserve">rodNpc2Default</t>
   </si>
   <si>
+    <t xml:space="preserve">rodNpc2Saved</t>
+  </si>
+  <si>
     <t xml:space="preserve">rodNpc3Win</t>
   </si>
   <si>
@@ -199,6 +211,9 @@
     <t xml:space="preserve">rodNpc3Default</t>
   </si>
   <si>
+    <t xml:space="preserve">rodNpc3Saved</t>
+  </si>
+  <si>
     <t xml:space="preserve">rodNpc4Win</t>
   </si>
   <si>
@@ -226,6 +241,9 @@
     <t xml:space="preserve">rodNpc4Default</t>
   </si>
   <si>
+    <t xml:space="preserve">rodNpc4Saved</t>
+  </si>
+  <si>
     <t xml:space="preserve">rodNpc5Win</t>
   </si>
   <si>
@@ -250,6 +268,9 @@
     <t xml:space="preserve">rodNpc5Default</t>
   </si>
   <si>
+    <t xml:space="preserve">rodNpc5Saved</t>
+  </si>
+  <si>
     <t xml:space="preserve">rodNpc6Win</t>
   </si>
   <si>
@@ -262,18 +283,18 @@
     <t xml:space="preserve">Yep 2/1 is 48 great work.</t>
   </si>
   <si>
+    <t xml:space="preserve">rodNpc6Fail</t>
+  </si>
+  <si>
     <t xml:space="preserve">scriptevent rod:npcComplete 6</t>
   </si>
   <si>
-    <t xml:space="preserve">rodNpc6Fail</t>
+    <t xml:space="preserve">rodNpc6Default</t>
   </si>
   <si>
     <t xml:space="preserve">scriptevent rod:npcReplay 6</t>
   </si>
   <si>
-    <t xml:space="preserve">rodNpc6Default</t>
-  </si>
-  <si>
     <t xml:space="preserve">rodNpc7Win</t>
   </si>
   <si>
@@ -286,18 +307,18 @@
     <t xml:space="preserve">Three is indeed 1/8 of 24.</t>
   </si>
   <si>
+    <t xml:space="preserve">rodNpc7Fail</t>
+  </si>
+  <si>
     <t xml:space="preserve">scriptevent rod:npcComplete 7</t>
   </si>
   <si>
-    <t xml:space="preserve">rodNpc7Fail</t>
+    <t xml:space="preserve">rodNpc7Default</t>
   </si>
   <si>
     <t xml:space="preserve">scriptevent rod:npcReplay 7</t>
   </si>
   <si>
-    <t xml:space="preserve">rodNpc7Default</t>
-  </si>
-  <si>
     <t xml:space="preserve">rodNpc8Win</t>
   </si>
   <si>
@@ -310,18 +331,18 @@
     <t xml:space="preserve">Great work you simplified 2/8 to 1/4.</t>
   </si>
   <si>
+    <t xml:space="preserve">rodNpc8Fail</t>
+  </si>
+  <si>
     <t xml:space="preserve">scriptevent rod:npcComplete 8</t>
   </si>
   <si>
-    <t xml:space="preserve">rodNpc8Fail</t>
+    <t xml:space="preserve">rodNpc8Default</t>
   </si>
   <si>
     <t xml:space="preserve">scriptevent rod:npcReplay 8</t>
   </si>
   <si>
-    <t xml:space="preserve">rodNpc8Default</t>
-  </si>
-  <si>
     <t xml:space="preserve">rodNpc9Win</t>
   </si>
   <si>
@@ -334,18 +355,18 @@
     <t xml:space="preserve">Two is 1/12 of24</t>
   </si>
   <si>
+    <t xml:space="preserve">rodNpc9Fail</t>
+  </si>
+  <si>
     <t xml:space="preserve">scriptevent rod:npcComplete 9</t>
   </si>
   <si>
-    <t xml:space="preserve">rodNpc9Fail</t>
+    <t xml:space="preserve">rodNpc9Default</t>
   </si>
   <si>
     <t xml:space="preserve">scriptevent rod:npcReplay 9</t>
   </si>
   <si>
-    <t xml:space="preserve">rodNpc9Default</t>
-  </si>
-  <si>
     <t xml:space="preserve">rodNpc10Win</t>
   </si>
   <si>
@@ -358,18 +379,18 @@
     <t xml:space="preserve">Great work simplifying the fraction from 2/12 to 1/6.</t>
   </si>
   <si>
+    <t xml:space="preserve">rodNpc10Fail</t>
+  </si>
+  <si>
     <t xml:space="preserve">scriptevent rod:npcComplete 10</t>
   </si>
   <si>
-    <t xml:space="preserve">rodNpc10Fail</t>
+    <t xml:space="preserve">rodNpc10Default</t>
   </si>
   <si>
     <t xml:space="preserve">scriptevent rod:npcReplay 10</t>
   </si>
   <si>
-    <t xml:space="preserve">rodNpc10Default</t>
-  </si>
-  <si>
     <t xml:space="preserve">rodNpc11Win</t>
   </si>
   <si>
@@ -382,21 +403,21 @@
     <t xml:space="preserve">You’ve done very well to get to me! I thought I was never going to be saved.</t>
   </si>
   <si>
+    <t xml:space="preserve">rodNpc11Fail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I won’t ever say this, if you see this something has gone wrong!</t>
+  </si>
+  <si>
     <t xml:space="preserve">scriptevent rod:npcComplete 11</t>
   </si>
   <si>
-    <t xml:space="preserve">rodNpc11Fail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I won’t ever say this, if you see this something has gone wrong!</t>
+    <t xml:space="preserve">rodNpc11Default</t>
   </si>
   <si>
     <t xml:space="preserve">scriptevent rod:npcReplay 11</t>
   </si>
   <si>
-    <t xml:space="preserve">rodNpc11Default</t>
-  </si>
-  <si>
     <t xml:space="preserve">rodNpc12Win</t>
   </si>
   <si>
@@ -409,19 +430,19 @@
     <t xml:space="preserve">Well done you saved us all!</t>
   </si>
   <si>
+    <t xml:space="preserve">rodNpc12Fail</t>
+  </si>
+  <si>
     <t xml:space="preserve">Thanks</t>
   </si>
   <si>
     <t xml:space="preserve">scriptevent rod:npcComplete 12</t>
   </si>
   <si>
-    <t xml:space="preserve">rodNpc12Fail</t>
+    <t xml:space="preserve">rodNpc12Default</t>
   </si>
   <si>
     <t xml:space="preserve">scriptevent rod:npcReplay 12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc12Default</t>
   </si>
 </sst>
 </file>
@@ -739,10 +760,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R87"/>
+  <dimension ref="A1:R94"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G7" colorId="64" zoomScale="109" zoomScaleNormal="109" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H42" activeCellId="0" sqref="H42"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="109" zoomScaleNormal="109" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A47" activeCellId="0" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -889,222 +910,215 @@
         <v>32</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="G5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>37</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="H5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="H6" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="G7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H7" s="3"/>
-    </row>
-    <row r="8" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" s="4" t="s">
+      <c r="G9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H8" s="3" t="s">
+      <c r="B10" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H9" s="3" t="s">
+      <c r="G10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H10" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="I9" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="G11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="I11" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="B12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H11" s="3" t="s">
+      <c r="B13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="3"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H12" s="3" t="s">
+      <c r="C14" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="D14" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H13" s="3"/>
-    </row>
-    <row r="14" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="G14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H14" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>26</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>28</v>
@@ -1112,13 +1126,13 @@
     </row>
     <row r="16" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>30</v>
@@ -1130,602 +1144,699 @@
     </row>
     <row r="17" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H18" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B17" s="1" t="s">
+    </row>
+    <row r="19" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="B19" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="G19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H19" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H17" s="3" t="s">
+      <c r="I19" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
+      <c r="B20" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H20" s="3"/>
+    </row>
+    <row r="21" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="G18" s="1" t="s">
+      <c r="B21" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H21" s="3"/>
+    </row>
+    <row r="22" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H18" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="I18" s="1" t="s">
+      <c r="H23" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="I23" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
+    <row r="24" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D19" s="1" t="s">
+      <c r="C24" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="G24" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H19" s="3"/>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
+      <c r="H24" s="3"/>
+    </row>
+    <row r="25" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
+      <c r="D25" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H25" s="3"/>
+    </row>
+    <row r="26" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H22" s="3"/>
-    </row>
-    <row r="23" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
+      <c r="B26" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="D26" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="H26" s="3"/>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="G23" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H23" s="3" t="s">
+      <c r="B27" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H27" s="3" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
+    <row r="28" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B28" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H25" s="3"/>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>30</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H28" s="3"/>
+        <v>26</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>31</v>
+      </c>
+      <c r="H29" s="3"/>
+    </row>
+    <row r="30" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>30</v>
       </c>
       <c r="G31" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="G32" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H31" s="3"/>
-    </row>
-    <row r="32" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H32" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="H32" s="3"/>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>30</v>
       </c>
       <c r="G34" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="G35" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H34" s="3"/>
-    </row>
-    <row r="35" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H35" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H35" s="3"/>
+    </row>
+    <row r="36" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>122</v>
+        <v>51</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>30</v>
       </c>
       <c r="G37" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="G38" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H37" s="3"/>
-    </row>
-    <row r="38" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="H38" s="3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="H38" s="3"/>
+    </row>
+    <row r="39" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>122</v>
+        <v>117</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="I39" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>30</v>
       </c>
       <c r="G40" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="G41" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H40" s="3"/>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D41" s="4"/>
-    </row>
-    <row r="42" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D42" s="4"/>
+      <c r="H41" s="3"/>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D43" s="4"/>
+      <c r="A43" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D44" s="4"/>
-    </row>
-    <row r="45" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D45" s="4"/>
+      <c r="A44" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H44" s="3"/>
+    </row>
+    <row r="45" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D46" s="4"/>
-    </row>
-    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D47" s="4"/>
-    </row>
-    <row r="48" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G47" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H47" s="3"/>
+    </row>
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D48" s="4"/>
     </row>
-    <row r="49" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D49" s="4"/>
     </row>
-    <row r="50" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D50" s="4"/>
     </row>
-    <row r="51" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D51" s="4"/>
     </row>
-    <row r="52" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D52" s="4"/>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D53" s="4"/>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D54" s="4"/>
     </row>
-    <row r="55" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D55" s="4"/>
     </row>
-    <row r="56" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D56" s="4"/>
     </row>
-    <row r="57" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D57" s="4"/>
     </row>
-    <row r="58" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D58" s="4"/>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D59" s="4"/>
     </row>
-    <row r="60" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D60" s="4"/>
     </row>
-    <row r="61" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D61" s="4"/>
     </row>
-    <row r="62" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D62" s="4"/>
     </row>
-    <row r="63" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D63" s="4"/>
     </row>
     <row r="64" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D64" s="4"/>
     </row>
-    <row r="65" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D65" s="4"/>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D66" s="4"/>
     </row>
-    <row r="67" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D67" s="4"/>
     </row>
-    <row r="68" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D68" s="4"/>
     </row>
-    <row r="69" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D69" s="4"/>
     </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D70" s="4"/>
     </row>
-    <row r="71" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D71" s="4"/>
     </row>
-    <row r="72" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D72" s="4"/>
     </row>
-    <row r="73" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D73" s="4"/>
     </row>
-    <row r="74" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D74" s="4"/>
     </row>
-    <row r="75" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D75" s="4"/>
-      <c r="J75" s="6"/>
-    </row>
-    <row r="76" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="76" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D76" s="4"/>
     </row>
-    <row r="77" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D77" s="4"/>
     </row>
     <row r="78" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1736,41 +1847,62 @@
     </row>
     <row r="80" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D80" s="4"/>
-      <c r="J80" s="6"/>
     </row>
     <row r="81" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D81" s="4"/>
-      <c r="J81" s="6"/>
     </row>
     <row r="82" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D82" s="4"/>
       <c r="J82" s="6"/>
     </row>
     <row r="83" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J83" s="6"/>
+      <c r="D83" s="4"/>
     </row>
     <row r="84" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J84" s="6"/>
+      <c r="D84" s="4"/>
     </row>
     <row r="85" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D85" s="4"/>
-      <c r="J85" s="6"/>
     </row>
     <row r="86" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D86" s="4"/>
-      <c r="J86" s="6"/>
     </row>
     <row r="87" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A87" s="7"/>
-      <c r="B87" s="7"/>
-      <c r="C87" s="7"/>
-      <c r="D87" s="7"/>
-      <c r="E87" s="7"/>
-      <c r="F87" s="7"/>
-      <c r="I87" s="7"/>
-      <c r="J87" s="7"/>
-      <c r="K87" s="7"/>
-      <c r="L87" s="7"/>
+      <c r="D87" s="4"/>
+      <c r="J87" s="6"/>
+    </row>
+    <row r="88" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D88" s="4"/>
+      <c r="J88" s="6"/>
+    </row>
+    <row r="89" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="J89" s="6"/>
+    </row>
+    <row r="90" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="J90" s="6"/>
+    </row>
+    <row r="91" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D91" s="4"/>
+      <c r="J91" s="6"/>
+    </row>
+    <row r="92" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D92" s="4"/>
+      <c r="J92" s="6"/>
+    </row>
+    <row r="93" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A93" s="7"/>
+      <c r="B93" s="7"/>
+      <c r="C93" s="7"/>
+      <c r="D93" s="7"/>
+      <c r="J93" s="6"/>
+    </row>
+    <row r="94" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E94" s="7"/>
+      <c r="F94" s="7"/>
+      <c r="I94" s="7"/>
+      <c r="J94" s="7"/>
+      <c r="K94" s="7"/>
+      <c r="L94" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
fixed issue with the window breaking
</commit_message>
<xml_diff>
--- a/npc/npc.xlsx
+++ b/npc/npc.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="164">
   <si>
     <t xml:space="preserve">Scene</t>
   </si>
@@ -430,12 +430,12 @@
     <t xml:space="preserve">Well done you saved us all!</t>
   </si>
   <si>
+    <t xml:space="preserve">Thanks</t>
+  </si>
+  <si>
     <t xml:space="preserve">rodNpc12Fail</t>
   </si>
   <si>
-    <t xml:space="preserve">Thanks</t>
-  </si>
-  <si>
     <t xml:space="preserve">scriptevent rod:npcComplete 12</t>
   </si>
   <si>
@@ -443,6 +443,75 @@
   </si>
   <si>
     <t xml:space="preserve">scriptevent rod:npcReplay 12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spawnNpc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Welcome! What challenge do you want to take on today?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fraction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scriptevent spawnNpc fraction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ratios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scriptevent spawnNpc ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scale Factors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scriptevent spawnNpc scale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scaleNpc0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scaleNpc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guild Master</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I need the help of a mathmogician to build some windows follow me!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Okay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ratioNpc0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ratioNpc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Professor of Alchemy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I’m hungry I’ve dropped my lunch money down the well, will you help?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For sure!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fractionNpc0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fractionNpc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Professor of Cartography</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is embarrassing, I’ve lost my cartography class in the walled gardens and need your help!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On my way!</t>
   </si>
 </sst>
 </file>
@@ -762,8 +831,8 @@
   </sheetPr>
   <dimension ref="A1:R94"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="109" zoomScaleNormal="109" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A47" activeCellId="0" sqref="A47"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K26" colorId="64" zoomScale="109" zoomScaleNormal="109" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L47" activeCellId="0" sqref="L47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1331,6 +1400,9 @@
       <c r="D26" s="4" t="s">
         <v>86</v>
       </c>
+      <c r="G26" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="H26" s="3"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1347,7 +1419,7 @@
         <v>51</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>88</v>
@@ -1367,7 +1439,7 @@
         <v>30</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>90</v>
@@ -1390,7 +1462,7 @@
         <v>94</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="H29" s="3"/>
     </row>
@@ -1408,7 +1480,7 @@
         <v>51</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="H30" s="3" t="s">
         <v>96</v>
@@ -1428,7 +1500,7 @@
         <v>30</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="H31" s="3" t="s">
         <v>98</v>
@@ -1451,7 +1523,7 @@
         <v>102</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="H32" s="3"/>
     </row>
@@ -1469,7 +1541,7 @@
         <v>51</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="H33" s="3" t="s">
         <v>104</v>
@@ -1489,7 +1561,7 @@
         <v>30</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="H34" s="3" t="s">
         <v>106</v>
@@ -1512,7 +1584,7 @@
         <v>110</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="H35" s="3"/>
     </row>
@@ -1530,7 +1602,7 @@
         <v>51</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="H36" s="3" t="s">
         <v>112</v>
@@ -1550,7 +1622,7 @@
         <v>30</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="H37" s="3" t="s">
         <v>114</v>
@@ -1573,7 +1645,7 @@
         <v>118</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="H38" s="3"/>
     </row>
@@ -1591,7 +1663,7 @@
         <v>51</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="H39" s="3" t="s">
         <v>120</v>
@@ -1611,7 +1683,7 @@
         <v>30</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="H40" s="3" t="s">
         <v>122</v>
@@ -1634,7 +1706,7 @@
         <v>126</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="H41" s="3"/>
     </row>
@@ -1652,7 +1724,7 @@
         <v>128</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="H42" s="3" t="s">
         <v>129</v>
@@ -1672,7 +1744,7 @@
         <v>30</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="H43" s="3" t="s">
         <v>131</v>
@@ -1695,13 +1767,13 @@
         <v>135</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>31</v>
+        <v>136</v>
       </c>
       <c r="H44" s="3"/>
     </row>
     <row r="45" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>133</v>
@@ -1713,7 +1785,7 @@
         <v>128</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>137</v>
+        <v>26</v>
       </c>
       <c r="H45" s="3" t="s">
         <v>138</v>
@@ -1733,7 +1805,7 @@
         <v>30</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="H46" s="3" t="s">
         <v>140</v>
@@ -1743,20 +1815,87 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D47" s="4"/>
+      <c r="A47" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>142</v>
+      </c>
       <c r="G47" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H47" s="3"/>
+        <v>143</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="L47" s="1" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D48" s="4"/>
+      <c r="A48" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D49" s="4"/>
-    </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D50" s="4"/>
+      <c r="A49" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="25.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D51" s="4"/>

</xml_diff>

<commit_message>
Fixed carrot ratio issue
</commit_message>
<xml_diff>
--- a/npc/npc.xlsx
+++ b/npc/npc.xlsx
@@ -454,19 +454,19 @@
     <t xml:space="preserve">Fraction</t>
   </si>
   <si>
-    <t xml:space="preserve">scriptevent spawnNpc fraction</t>
+    <t xml:space="preserve">scriptevent spawn:npc fraction</t>
   </si>
   <si>
     <t xml:space="preserve">Ratios</t>
   </si>
   <si>
-    <t xml:space="preserve">scriptevent spawnNpc ratio</t>
+    <t xml:space="preserve">scriptevent spawn:npc ratio</t>
   </si>
   <si>
     <t xml:space="preserve">Scale Factors</t>
   </si>
   <si>
-    <t xml:space="preserve">scriptevent spawnNpc scale</t>
+    <t xml:space="preserve">scriptevent spawn:npc scale</t>
   </si>
   <si>
     <t xml:space="preserve">scaleNpc0</t>
@@ -831,8 +831,8 @@
   </sheetPr>
   <dimension ref="A1:R94"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G24" colorId="64" zoomScale="109" zoomScaleNormal="109" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J47" activeCellId="0" sqref="J47"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H34" colorId="64" zoomScale="109" zoomScaleNormal="109" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L47" activeCellId="0" sqref="L47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Added dialogue changing to npcWalk
</commit_message>
<xml_diff>
--- a/npc/npc.xlsx
+++ b/npc/npc.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="174">
   <si>
     <t xml:space="preserve">Scene</t>
   </si>
@@ -485,6 +485,27 @@
   </si>
   <si>
     <t xml:space="preserve">scriptevent scale:npc 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scaleNpc1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep up, keep up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sorry! </t>
+  </si>
+  <si>
+    <t xml:space="preserve">scaleNpc2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Take this stained glass and place it in the smaller frames, when you’re ready left click the numerator to increase scaling amount. Then right click the fraction bar to scale the window.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Will do</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scriptevent scale:npc 1</t>
   </si>
   <si>
     <t xml:space="preserve">ratioNpc0</t>
@@ -840,8 +861,8 @@
   </sheetPr>
   <dimension ref="A1:R94"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G31" colorId="64" zoomScale="109" zoomScaleNormal="109" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I50" activeCellId="0" sqref="I50"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="109" zoomScaleNormal="109" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B54" activeCellId="0" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1880,46 +1901,81 @@
         <v>155</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="G49" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="D49" s="4" t="s">
+    </row>
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="G49" s="1" t="s">
+      <c r="B50" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="H49" s="3" t="s">
+      <c r="G50" s="1" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="50" customFormat="false" ht="25.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1" t="s">
+      <c r="H50" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B50" s="1" t="s">
+    </row>
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="B51" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="D50" s="4" t="s">
+      <c r="C51" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="G50" s="1" t="s">
+      <c r="D51" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="H50" s="3" t="s">
+      <c r="G51" s="1" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D51" s="4"/>
+      <c r="H51" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="I51" s="0"/>
+      <c r="J51" s="0"/>
     </row>
     <row r="52" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D52" s="4"/>
+      <c r="A52" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="H52" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="I52" s="0"/>
+      <c r="J52" s="0"/>
     </row>
     <row r="53" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D53" s="4"/>
@@ -1933,12 +1989,8 @@
     <row r="56" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D56" s="4"/>
     </row>
-    <row r="57" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D57" s="4"/>
-    </row>
-    <row r="58" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D58" s="4"/>
-    </row>
+    <row r="57" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="58" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="59" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D59" s="4"/>
     </row>

</xml_diff>

<commit_message>
Added the  first parts of the npc's
</commit_message>
<xml_diff>
--- a/npc/npc.xlsx
+++ b/npc/npc.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="188">
   <si>
     <t xml:space="preserve">Scene</t>
   </si>
@@ -490,7 +490,7 @@
     <t xml:space="preserve">scaleNpc1</t>
   </si>
   <si>
-    <t xml:space="preserve">Keep up, keep up</t>
+    <t xml:space="preserve">Keep up, keep up.</t>
   </si>
   <si>
     <t xml:space="preserve">Sorry! </t>
@@ -526,6 +526,27 @@
     <t xml:space="preserve">scriptevent ratio:npc 0</t>
   </si>
   <si>
+    <t xml:space="preserve">ratioNpc1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please hurry, I’m so hungry.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I’m on my way.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ratioNpc2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Here is the well, you’ll need potions to dive deeper and see in the dark. My students have put the ratios you’ll need to make the potions on the wall. Take these ingredients and throw them in the hopper to make the potions.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Okay I’m on it. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">scriptevent ratio:npc 1</t>
+  </si>
+  <si>
     <t xml:space="preserve">fractionNpc0</t>
   </si>
   <si>
@@ -542,6 +563,27 @@
   </si>
   <si>
     <t xml:space="preserve">scriptevent fraction:npc 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fractionNpc1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oh dear oh dear, please keep up I cannot lose a whole class.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sorry I’ll keep up!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fractionNpc2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Take these magical rods you’ll be able to cross the garden without stepping on the grass. You;ll need to work out the fractions to cross the gaps in the garden.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wish me luck</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scriptevent fraction:npc 1</t>
   </si>
 </sst>
 </file>
@@ -551,13 +593,13 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
-      <charset val="134"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -577,13 +619,6 @@
     <font>
       <sz val="16"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
@@ -643,7 +678,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -656,20 +691,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -861,8 +888,8 @@
   </sheetPr>
   <dimension ref="A1:R94"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="109" zoomScaleNormal="109" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B54" activeCellId="0" sqref="B54"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A32" colorId="64" zoomScale="109" zoomScaleNormal="109" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H67" activeCellId="0" sqref="H67:H69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1811,7 +1838,7 @@
       <c r="C45" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="D45" s="4" t="s">
         <v>128</v>
       </c>
       <c r="G45" s="1" t="s">
@@ -1952,42 +1979,100 @@
       <c r="H51" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="I51" s="0"/>
-      <c r="J51" s="0"/>
     </row>
     <row r="52" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B52" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="G52" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="D52" s="4" t="s">
+    </row>
+    <row r="53" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="G52" s="1" t="s">
+      <c r="B53" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D53" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="H52" s="3" t="s">
+      <c r="G53" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="I52" s="0"/>
-      <c r="J52" s="0"/>
-    </row>
-    <row r="53" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D53" s="4"/>
+      <c r="H53" s="1" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D54" s="4"/>
+      <c r="A54" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="H54" s="3" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D55" s="4"/>
+      <c r="A55" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D56" s="4"/>
+      <c r="A56" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="58" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2062,7 +2147,7 @@
     </row>
     <row r="82" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D82" s="4"/>
-      <c r="J82" s="6"/>
+      <c r="J82" s="3"/>
     </row>
     <row r="83" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D83" s="4"/>
@@ -2078,40 +2163,40 @@
     </row>
     <row r="87" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D87" s="4"/>
-      <c r="J87" s="6"/>
+      <c r="J87" s="3"/>
     </row>
     <row r="88" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D88" s="4"/>
-      <c r="J88" s="6"/>
+      <c r="J88" s="3"/>
     </row>
     <row r="89" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J89" s="6"/>
+      <c r="J89" s="3"/>
     </row>
     <row r="90" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J90" s="6"/>
+      <c r="J90" s="3"/>
     </row>
     <row r="91" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D91" s="4"/>
-      <c r="J91" s="6"/>
+      <c r="J91" s="3"/>
     </row>
     <row r="92" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D92" s="4"/>
-      <c r="J92" s="6"/>
+      <c r="J92" s="3"/>
     </row>
     <row r="93" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A93" s="7"/>
-      <c r="B93" s="7"/>
-      <c r="C93" s="7"/>
-      <c r="D93" s="7"/>
-      <c r="J93" s="6"/>
+      <c r="A93" s="5"/>
+      <c r="B93" s="5"/>
+      <c r="C93" s="5"/>
+      <c r="D93" s="5"/>
+      <c r="J93" s="3"/>
     </row>
     <row r="94" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E94" s="7"/>
-      <c r="F94" s="7"/>
-      <c r="I94" s="7"/>
-      <c r="J94" s="7"/>
-      <c r="K94" s="7"/>
-      <c r="L94" s="7"/>
+      <c r="E94" s="5"/>
+      <c r="F94" s="5"/>
+      <c r="I94" s="5"/>
+      <c r="J94" s="5"/>
+      <c r="K94" s="5"/>
+      <c r="L94" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Added grroff my grass
</commit_message>
<xml_diff>
--- a/npc/npc.xlsx
+++ b/npc/npc.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="191">
   <si>
     <t xml:space="preserve">Scene</t>
   </si>
@@ -583,7 +583,16 @@
     <t xml:space="preserve">Wish me luck</t>
   </si>
   <si>
-    <t xml:space="preserve">scriptevent fraction:npc 1</t>
+    <t xml:space="preserve">groundskeeper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grumpy Groundskeeper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grrrrofffff me grass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tp @p 30 96 107 facing 30 96 90</t>
   </si>
 </sst>
 </file>
@@ -593,7 +602,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -622,6 +631,12 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="4">
@@ -678,7 +693,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -697,6 +712,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -888,8 +907,8 @@
   </sheetPr>
   <dimension ref="A1:R94"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A32" colorId="64" zoomScale="109" zoomScaleNormal="109" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H67" activeCellId="0" sqref="H67:H69"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E40" colorId="64" zoomScale="109" zoomScaleNormal="109" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H57" activeCellId="0" sqref="H57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2070,11 +2089,33 @@
       <c r="G56" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="H56" s="1" t="s">
+    </row>
+    <row r="57" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="57" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="B57" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="H57" s="5" t="s">
+        <v>190</v>
+      </c>
+    </row>
     <row r="58" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="59" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D59" s="4"/>
@@ -2184,19 +2225,19 @@
       <c r="J92" s="3"/>
     </row>
     <row r="93" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A93" s="5"/>
-      <c r="B93" s="5"/>
-      <c r="C93" s="5"/>
-      <c r="D93" s="5"/>
+      <c r="A93" s="6"/>
+      <c r="B93" s="6"/>
+      <c r="C93" s="6"/>
+      <c r="D93" s="6"/>
       <c r="J93" s="3"/>
     </row>
     <row r="94" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E94" s="5"/>
-      <c r="F94" s="5"/>
-      <c r="I94" s="5"/>
-      <c r="J94" s="5"/>
-      <c r="K94" s="5"/>
-      <c r="L94" s="5"/>
+      <c r="E94" s="6"/>
+      <c r="F94" s="6"/>
+      <c r="I94" s="6"/>
+      <c r="J94" s="6"/>
+      <c r="K94" s="6"/>
+      <c r="L94" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
added rods back into npc
</commit_message>
<xml_diff>
--- a/npc/npc.xlsx
+++ b/npc/npc.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="192">
   <si>
     <t xml:space="preserve">Scene</t>
   </si>
@@ -581,6 +581,9 @@
   </si>
   <si>
     <t xml:space="preserve">Wish me luck</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scriptevent fraction:npc 1</t>
   </si>
   <si>
     <t xml:space="preserve">groundskeeper</t>
@@ -602,7 +605,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -631,12 +634,6 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="4">
@@ -693,7 +690,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -712,10 +709,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -908,7 +901,7 @@
   <dimension ref="A1:R94"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E40" colorId="64" zoomScale="109" zoomScaleNormal="109" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H57" activeCellId="0" sqref="H57"/>
+      <selection pane="topLeft" activeCell="H56" activeCellId="0" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2089,31 +2082,34 @@
       <c r="G56" s="1" t="s">
         <v>186</v>
       </c>
+      <c r="H56" s="1" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="F57" s="5" t="s">
-        <v>190</v>
+        <v>191</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>191</v>
       </c>
       <c r="G57" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="H57" s="5" t="s">
-        <v>190</v>
+      <c r="H57" s="3" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2225,19 +2221,19 @@
       <c r="J92" s="3"/>
     </row>
     <row r="93" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A93" s="6"/>
-      <c r="B93" s="6"/>
-      <c r="C93" s="6"/>
-      <c r="D93" s="6"/>
+      <c r="A93" s="5"/>
+      <c r="B93" s="5"/>
+      <c r="C93" s="5"/>
+      <c r="D93" s="5"/>
       <c r="J93" s="3"/>
     </row>
     <row r="94" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E94" s="6"/>
-      <c r="F94" s="6"/>
-      <c r="I94" s="6"/>
-      <c r="J94" s="6"/>
-      <c r="K94" s="6"/>
-      <c r="L94" s="6"/>
+      <c r="E94" s="5"/>
+      <c r="F94" s="5"/>
+      <c r="I94" s="5"/>
+      <c r="J94" s="5"/>
+      <c r="K94" s="5"/>
+      <c r="L94" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
ratio update based on Bryans feedback
</commit_message>
<xml_diff>
--- a/npc/npc.xlsx
+++ b/npc/npc.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="199">
   <si>
     <t xml:space="preserve">Scene</t>
   </si>
@@ -517,43 +517,81 @@
     <t xml:space="preserve">Professor of Alchemy</t>
   </si>
   <si>
-    <t xml:space="preserve">I need your help! I am so hungry, but clumsy me managed to drop my lunch money down the well. Please follow me and use maths to get my money back!</t>
+    <t xml:space="preserve">I see you want to take on the Well diving championship, very well, follow me. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Let's Go</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scriptevent ratio:npc 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ratioNpc1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The challenge awaits, please keep up.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On the way!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ratioNpc2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Here take these ingredients, come back if you need anymore.
+The ratios for the ingredients are on the wall. 
+To make a potion mix it in the cauldron and tap it with your wand.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thank you</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scriptevent ratio:npc 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ratioNpc3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How can I help</t>
+  </si>
+  <si>
+    <t xml:space="preserve">More ingredients please</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scriptevent ratio:npc 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I’m stuck</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dialogue open @e[tag=ratioNpc] @p ratioNpc4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ratioNpc4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Here are the steps for the game. 
+1. Check the ratios on the wall.
+2. Chuck the ingredients in the cauldron to the correct ratio.
+3. Click on the cauldron with your wand.
+4. Check the bar chart to see if your ratios are correct. 
+5. If they are correct, drink the potion and dive in the well. 
+6. Remember to follow the rules and click on the coins to gather them. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">fractionNpc0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fractionNpc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Professor of Cartography</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is embarrassing, I’ve lost my cartography students in the walled gardens (yes I know). Please help me! Follow me to the gardens.</t>
   </si>
   <si>
     <t xml:space="preserve">Let's Go!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scriptevent ratio:npc 0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ratioNpc1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Please hurry, I’m so hungry.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">On the way!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ratioNpc2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The well is very dark and deep, you will need to make potions to see and breathe long enough to get my money back. Use the ratios on the walls to make two of the correct potions. Use the ingredients I am giving you and throw them in the hopper, then left click with the wand to make the potions. Be careful, if you get the wrong ratios there may be... side effects. Hint: If the potions you have made do not last long enough, you need to increase the ingredients. But remember as you add to make sure the ratios are still correct! We can't afford any more accidents, not on my watch.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scriptevent ratio:npc 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fractionNpc0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fractionNpc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Professor of Cartography</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is embarrassing, I’ve lost my cartography students in the walled gardens (yes I know). Please help me! Follow me to the gardens.</t>
   </si>
   <si>
     <t xml:space="preserve">scriptevent fraction:npc 0</t>
@@ -688,32 +726,36 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -900,1324 +942,1370 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R94"/>
+  <dimension ref="A1:R97"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="109" zoomScaleNormal="109" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D50" activeCellId="0" sqref="D50"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A36" colorId="64" zoomScale="109" zoomScaleNormal="109" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H55" activeCellId="0" sqref="H55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.16796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="82.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="38.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="24.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="20"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="44.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="22.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="29.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="23.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="82.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="38.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="18.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="18.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="41.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="20"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="10.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="44.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="22.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="29.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="23.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="4" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="I7" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="4" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="H11" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="I11" s="3" t="s">
+      <c r="I11" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G13" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G14" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="H14" s="4" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="H15" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="I15" s="3" t="s">
+      <c r="I15" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G16" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G17" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G18" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="H18" s="4" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="G19" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="H19" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="I19" s="3" t="s">
+      <c r="I19" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G20" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="G21" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="G22" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="H22" s="4" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="G23" s="3" t="s">
+      <c r="G23" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="H23" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="I23" s="3" t="s">
+      <c r="I23" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="C24" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="G24" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C25" s="0" t="s">
+      <c r="C25" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="G25" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C26" s="0" t="s">
+      <c r="C26" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="G26" s="3" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C27" s="0" t="s">
+      <c r="C27" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="G27" s="3" t="s">
+      <c r="G27" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H27" s="3" t="s">
+      <c r="H27" s="4" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B28" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="C28" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D28" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="G28" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H28" s="3" t="s">
+      <c r="H28" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="I28" s="3" t="s">
+      <c r="I28" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="A29" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="B29" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="G29" s="3" t="s">
+      <c r="G29" s="4" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G30" s="3" t="s">
+      <c r="G30" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H30" s="3" t="s">
+      <c r="H30" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="A31" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="B31" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D31" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G31" s="2" t="s">
+      <c r="G31" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H31" s="3" t="s">
+      <c r="H31" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="I31" s="3" t="s">
+      <c r="I31" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+      <c r="A32" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B32" s="0" t="s">
+      <c r="B32" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="G32" s="3" t="s">
+      <c r="G32" s="4" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="A33" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="B33" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D33" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G33" s="3" t="s">
+      <c r="G33" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H33" s="3" t="s">
+      <c r="H33" s="4" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="A34" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B34" s="0" t="s">
+      <c r="B34" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D34" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G34" s="2" t="s">
+      <c r="G34" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H34" s="3" t="s">
+      <c r="H34" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="I34" s="3" t="s">
+      <c r="I34" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+      <c r="A35" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B35" s="0" t="s">
+      <c r="B35" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D35" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="G35" s="3" t="s">
+      <c r="G35" s="4" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+      <c r="A36" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B36" s="0" t="s">
+      <c r="B36" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D36" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="G36" s="3" t="s">
+      <c r="G36" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H36" s="3" t="s">
+      <c r="H36" s="4" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+      <c r="A37" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B37" s="0" t="s">
+      <c r="B37" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C37" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D37" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G37" s="2" t="s">
+      <c r="G37" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H37" s="3" t="s">
+      <c r="H37" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="I37" s="3" t="s">
+      <c r="I37" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+      <c r="A38" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B38" s="0" t="s">
+      <c r="B38" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D38" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="G38" s="2" t="s">
+      <c r="G38" s="3" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+      <c r="A39" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B39" s="0" t="s">
+      <c r="B39" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C39" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="D39" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G39" s="3" t="s">
+      <c r="G39" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H39" s="3" t="s">
+      <c r="H39" s="4" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+      <c r="A40" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B40" s="0" t="s">
+      <c r="B40" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="D40" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G40" s="2" t="s">
+      <c r="G40" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H40" s="3" t="s">
+      <c r="H40" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="I40" s="3" t="s">
+      <c r="I40" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+      <c r="A41" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B41" s="0" t="s">
+      <c r="B41" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C41" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="D41" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="G41" s="3" t="s">
+      <c r="G41" s="4" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+      <c r="A42" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B42" s="0" t="s">
+      <c r="B42" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="D42" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="G42" s="3" t="s">
+      <c r="G42" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H42" s="3" t="s">
+      <c r="H42" s="4" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+      <c r="A43" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B43" s="0" t="s">
+      <c r="B43" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C43" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="D43" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G43" s="2" t="s">
+      <c r="G43" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H43" s="3" t="s">
+      <c r="H43" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="I43" s="3" t="s">
+      <c r="I43" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+      <c r="A44" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B44" s="0" t="s">
+      <c r="B44" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C44" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="D44" s="4" t="s">
+      <c r="D44" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="G44" s="3" t="s">
+      <c r="G44" s="4" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+      <c r="A45" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B45" s="0" t="s">
+      <c r="B45" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C45" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="D45" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="G45" s="3" t="s">
+      <c r="G45" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H45" s="3" t="s">
+      <c r="H45" s="4" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+      <c r="A46" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B46" s="0" t="s">
+      <c r="B46" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C46" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="D46" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E46" s="2" t="s">
+      <c r="E46" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="G46" s="2" t="s">
+      <c r="G46" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H46" s="3" t="s">
+      <c r="H46" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="I46" s="3" t="s">
+      <c r="I46" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="25.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+      <c r="A47" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B47" s="0" t="s">
+      <c r="B47" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C47" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="D47" s="4" t="s">
+      <c r="D47" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="G47" s="3" t="s">
+      <c r="G47" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="H47" s="3" t="s">
+      <c r="H47" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="I47" s="3" t="s">
+      <c r="I47" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="J47" s="3" t="s">
+      <c r="J47" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="K47" s="3" t="s">
+      <c r="K47" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="L47" s="3" t="s">
+      <c r="L47" s="4" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="25.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+      <c r="A48" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B48" s="0" t="s">
+      <c r="B48" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="C48" s="0" t="s">
+      <c r="C48" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="D48" s="4" t="s">
+      <c r="D48" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="G48" s="3" t="s">
+      <c r="G48" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="H48" s="3" t="s">
+      <c r="H48" s="4" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
+      <c r="A49" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B49" s="0" t="s">
+      <c r="B49" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="C49" s="0" t="s">
+      <c r="C49" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="D49" s="0" t="s">
+      <c r="D49" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="G49" s="0" t="s">
+      <c r="G49" s="1" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
+      <c r="A50" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B50" s="0" t="s">
+      <c r="B50" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="C50" s="0" t="s">
+      <c r="C50" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="D50" s="2" t="s">
+      <c r="D50" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="G50" s="3" t="s">
+      <c r="G50" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="H50" s="3" t="s">
+      <c r="H50" s="4" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="25.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
+    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B51" s="0" t="s">
+      <c r="B51" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="C51" s="0" t="s">
+      <c r="C51" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="D51" s="4" t="s">
+      <c r="D51" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="G51" s="2" t="s">
+      <c r="G51" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="H51" s="3" t="s">
+      <c r="H51" s="4" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
+      <c r="A52" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B52" s="0" t="s">
+      <c r="B52" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="C52" s="0" t="s">
+      <c r="C52" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="D52" s="0" t="s">
+      <c r="D52" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="G52" s="2" t="s">
+      <c r="G52" s="3" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
+      <c r="A53" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="B53" s="0" t="s">
+      <c r="B53" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="C53" s="0" t="s">
+      <c r="C53" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="D53" s="4" t="s">
+      <c r="D53" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="G53" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H53" s="3" t="s">
+      <c r="G53" s="3" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
+      <c r="H53" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="B54" s="0" t="s">
+    </row>
+    <row r="54" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="C54" s="0" t="s">
+      <c r="B54" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D54" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="D54" s="4" t="s">
+      <c r="G54" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="G54" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="H54" s="3" t="s">
+      <c r="H54" s="4" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="55" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
+      <c r="I54" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="B55" s="0" t="s">
-        <v>175</v>
-      </c>
-      <c r="C55" s="0" t="s">
-        <v>176</v>
+      <c r="J54" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>164</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="G55" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="H55" s="4"/>
+    </row>
+    <row r="56" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="H56" s="4" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="G57" s="3" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
-        <v>181</v>
-      </c>
-      <c r="B56" s="0" t="s">
-        <v>175</v>
-      </c>
-      <c r="C56" s="0" t="s">
-        <v>176</v>
-      </c>
-      <c r="D56" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="G56" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="H56" s="3" t="s">
+    <row r="58" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="57" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
+      <c r="C58" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B57" s="0" t="s">
-        <v>185</v>
-      </c>
-      <c r="C57" s="0" t="s">
-        <v>186</v>
-      </c>
-      <c r="D57" s="0" t="s">
-        <v>187</v>
-      </c>
-      <c r="E57" s="0" t="s">
-        <v>188</v>
-      </c>
-      <c r="F57" s="0" t="s">
-        <v>188</v>
-      </c>
-      <c r="G57" s="0" t="s">
+      <c r="D58" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="G58" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="H58" s="4" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="G59" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="H57" s="0" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="59" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C59" s="2"/>
-      <c r="D59" s="4"/>
-      <c r="G59" s="2"/>
-    </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C60" s="2"/>
-      <c r="D60" s="4"/>
-      <c r="G60" s="2"/>
-    </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C61" s="2"/>
-      <c r="D61" s="4"/>
-      <c r="G61" s="2"/>
-    </row>
-    <row r="62" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D62" s="4"/>
-    </row>
-    <row r="63" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C63" s="2"/>
-      <c r="D63" s="4"/>
-      <c r="G63" s="2"/>
-    </row>
-    <row r="64" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="H59" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="61" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C61" s="3"/>
+      <c r="D61" s="5"/>
+      <c r="G61" s="3"/>
+    </row>
+    <row r="62" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C62" s="3"/>
+      <c r="D62" s="5"/>
+      <c r="G62" s="3"/>
+    </row>
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C63" s="3"/>
+      <c r="D63" s="5"/>
+      <c r="G63" s="3"/>
+    </row>
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D64" s="5"/>
     </row>
-    <row r="65" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C65" s="3"/>
       <c r="D65" s="5"/>
-    </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D66" s="5"/>
-    </row>
-    <row r="67" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D67" s="5"/>
-    </row>
-    <row r="68" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D68" s="5"/>
-    </row>
-    <row r="69" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D69" s="5"/>
+      <c r="G65" s="3"/>
+    </row>
+    <row r="66" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D66" s="6"/>
+    </row>
+    <row r="67" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D67" s="6"/>
+    </row>
+    <row r="68" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D68" s="6"/>
+    </row>
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D69" s="6"/>
     </row>
     <row r="70" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D70" s="5"/>
-    </row>
-    <row r="71" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D71" s="5"/>
-    </row>
-    <row r="72" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D72" s="5"/>
-    </row>
-    <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D73" s="5"/>
-    </row>
-    <row r="74" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D74" s="5"/>
-    </row>
-    <row r="75" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D75" s="5"/>
-    </row>
-    <row r="76" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D76" s="5"/>
-    </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D77" s="5"/>
-    </row>
-    <row r="78" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D78" s="5"/>
-    </row>
-    <row r="79" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D79" s="5"/>
-    </row>
-    <row r="80" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D80" s="5"/>
+      <c r="D70" s="6"/>
+    </row>
+    <row r="71" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D71" s="6"/>
+    </row>
+    <row r="72" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D72" s="6"/>
+    </row>
+    <row r="73" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D73" s="6"/>
+    </row>
+    <row r="74" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D74" s="6"/>
+    </row>
+    <row r="75" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D75" s="6"/>
+    </row>
+    <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D76" s="6"/>
+    </row>
+    <row r="77" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D77" s="6"/>
+    </row>
+    <row r="78" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D78" s="6"/>
+    </row>
+    <row r="79" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D79" s="6"/>
+    </row>
+    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D80" s="6"/>
     </row>
     <row r="81" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D81" s="5"/>
+      <c r="D81" s="6"/>
     </row>
     <row r="82" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D82" s="5"/>
+      <c r="D82" s="6"/>
     </row>
     <row r="83" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D83" s="5"/>
+      <c r="D83" s="6"/>
     </row>
     <row r="84" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D84" s="5"/>
+      <c r="D84" s="6"/>
     </row>
     <row r="85" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D85" s="5"/>
+      <c r="D85" s="6"/>
     </row>
     <row r="86" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D86" s="5"/>
+      <c r="D86" s="6"/>
     </row>
     <row r="87" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D87" s="5"/>
+      <c r="D87" s="6"/>
     </row>
     <row r="88" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D88" s="5"/>
-    </row>
-    <row r="89" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="90" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="91" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D91" s="5"/>
-    </row>
-    <row r="92" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D92" s="5"/>
-    </row>
+      <c r="D88" s="6"/>
+    </row>
+    <row r="89" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D89" s="6"/>
+    </row>
+    <row r="90" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D90" s="6"/>
+    </row>
+    <row r="91" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="92" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="93" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A93" s="6"/>
-      <c r="B93" s="6"/>
-      <c r="C93" s="6"/>
       <c r="D93" s="6"/>
     </row>
     <row r="94" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E94" s="6"/>
-      <c r="F94" s="6"/>
-      <c r="I94" s="6"/>
-      <c r="J94" s="6"/>
-      <c r="K94" s="6"/>
-      <c r="L94" s="6"/>
+      <c r="D94" s="6"/>
+    </row>
+    <row r="95" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A95" s="7"/>
+      <c r="B95" s="7"/>
+      <c r="C95" s="7"/>
+      <c r="D95" s="7"/>
+    </row>
+    <row r="96" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E96" s="7"/>
+      <c r="F96" s="7"/>
+    </row>
+    <row r="97" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I97" s="7"/>
+      <c r="J97" s="7"/>
+      <c r="K97" s="7"/>
+      <c r="L97" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Added the warning that you've cheated
</commit_message>
<xml_diff>
--- a/npc/npc.xlsx
+++ b/npc/npc.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="201">
   <si>
     <t xml:space="preserve">Scene</t>
   </si>
@@ -517,7 +517,7 @@
     <t xml:space="preserve">Professor of Alchemy</t>
   </si>
   <si>
-    <t xml:space="preserve">I see you want to take on the Well diving championship, very well, follow me. </t>
+    <t xml:space="preserve">I hear you want to take on the Well diving championship, very well, follow me. </t>
   </si>
   <si>
     <t xml:space="preserve">Let's Go</t>
@@ -538,7 +538,7 @@
     <t xml:space="preserve">ratioNpc2</t>
   </si>
   <si>
-    <t xml:space="preserve">Here take these ingredients, come back if you need anymore.
+    <t xml:space="preserve">Here take these ingredients, come back if you need any more
 The ratios for the ingredients are on the wall. 
 To make a potion mix it in the cauldron and tap it with your wand.</t>
   </si>
@@ -579,6 +579,12 @@
 6. Remember to follow the rules and click on the coins to gather them. </t>
   </si>
   <si>
+    <t xml:space="preserve">ratioNpc5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You broke rule number 2, you must let the potions do the work, no swimming or diving.</t>
+  </si>
+  <si>
     <t xml:space="preserve">fractionNpc0</t>
   </si>
   <si>
@@ -591,40 +597,40 @@
     <t xml:space="preserve">This is embarrassing, I’ve lost my cartography students in the walled gardens (yes I know). Please help me! Follow me to the gardens.</t>
   </si>
   <si>
+    <t xml:space="preserve">fractionNpc1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oh dear oh dear, please keep up I cannot lose a whole class.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Let's Go!</t>
   </si>
   <si>
     <t xml:space="preserve">scriptevent fraction:npc 0</t>
   </si>
   <si>
-    <t xml:space="preserve">fractionNpc1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oh dear oh dear, please keep up I cannot lose a whole class.</t>
-  </si>
-  <si>
     <t xml:space="preserve">fractionNpc2</t>
   </si>
   <si>
     <t xml:space="preserve">I need you to rescue each student that is trapped. But you CANNOT touch the grass or the groundskeeper will get very angry. Use these magical rods to reach each student. You need to work out the fractions to get to the area correctly. If you make a mistake or touch the grass head back to me to start again. You can use the numbers on the walls to work out how far each student is, and therefore which rod to use! </t>
   </si>
   <si>
+    <t xml:space="preserve">groundskeeper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grumpy Groundskeeper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grrrrofffff me grass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tp @p 30 96 107 facing 30 96 90</t>
+  </si>
+  <si>
     <t xml:space="preserve">Wish me luck</t>
   </si>
   <si>
     <t xml:space="preserve">scriptevent fraction:npc 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">groundskeeper</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grumpy Groundskeeper</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grrrrofffff me grass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tp @p 30 96 107 facing 30 96 90</t>
   </si>
 </sst>
 </file>
@@ -942,10 +948,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R97"/>
+  <dimension ref="A1:R99"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A36" colorId="64" zoomScale="109" zoomScaleNormal="109" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H55" activeCellId="0" sqref="H55"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A33" colorId="64" zoomScale="109" zoomScaleNormal="109" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A61" activeCellId="0" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.16796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2102,128 +2108,146 @@
       <c r="H55" s="4"/>
     </row>
     <row r="56" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="6" t="s">
+      <c r="A56" s="1" t="s">
         <v>183</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D56" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="G56" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="H56" s="4"/>
+    </row>
+    <row r="57" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="D56" s="5" t="s">
+      <c r="B57" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="G56" s="3" t="s">
+      <c r="C57" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="H56" s="4" t="s">
+      <c r="D57" s="5" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="1" t="s">
+      <c r="G57" s="3"/>
+      <c r="H57" s="4"/>
+    </row>
+    <row r="58" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B57" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D57" s="6" t="s">
+      <c r="B58" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D58" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="G57" s="3" t="s">
+      <c r="G58" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="H58" s="4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="G59" s="3" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="G58" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="H58" s="4" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="1" t="s">
+    <row r="60" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B60" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C60" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="D60" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="E59" s="1" t="s">
+      <c r="E60" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="F59" s="1" t="s">
+      <c r="F60" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="G59" s="1" t="s">
+      <c r="G60" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="H60" s="4" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G61" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="H59" s="1" t="s">
+      <c r="H61" s="1" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="60" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="61" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C61" s="3"/>
-      <c r="D61" s="5"/>
-      <c r="G61" s="3"/>
     </row>
     <row r="62" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C62" s="3"/>
       <c r="D62" s="5"/>
-      <c r="G62" s="3"/>
-    </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="63" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C63" s="3"/>
       <c r="D63" s="5"/>
       <c r="G63" s="3"/>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C64" s="3"/>
       <c r="D64" s="5"/>
-    </row>
-    <row r="65" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C65" s="3"/>
+      <c r="G64" s="3"/>
+    </row>
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D65" s="5"/>
       <c r="G65" s="3"/>
     </row>
-    <row r="66" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D66" s="6"/>
-    </row>
-    <row r="67" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C66" s="3"/>
+      <c r="D66" s="5"/>
+    </row>
+    <row r="67" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D67" s="6"/>
-    </row>
-    <row r="68" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G67" s="3"/>
+    </row>
+    <row r="68" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D68" s="6"/>
     </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D69" s="6"/>
     </row>
-    <row r="70" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D70" s="6"/>
     </row>
-    <row r="71" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D71" s="6"/>
     </row>
     <row r="72" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2232,31 +2256,31 @@
     <row r="73" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D73" s="6"/>
     </row>
-    <row r="74" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D74" s="6"/>
     </row>
-    <row r="75" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D75" s="6"/>
     </row>
-    <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D76" s="6"/>
     </row>
     <row r="77" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D77" s="6"/>
     </row>
-    <row r="78" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D78" s="6"/>
     </row>
     <row r="79" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D79" s="6"/>
     </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D80" s="6"/>
     </row>
-    <row r="81" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D81" s="6"/>
     </row>
-    <row r="82" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D82" s="6"/>
     </row>
     <row r="83" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2283,29 +2307,33 @@
     <row r="90" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D90" s="6"/>
     </row>
-    <row r="91" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="91" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D91" s="6"/>
+    </row>
     <row r="92" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="93" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D93" s="6"/>
-    </row>
+    <row r="93" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="94" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D94" s="6"/>
     </row>
     <row r="95" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A95" s="7"/>
-      <c r="B95" s="7"/>
-      <c r="C95" s="7"/>
-      <c r="D95" s="7"/>
+      <c r="D95" s="6"/>
     </row>
     <row r="96" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E96" s="7"/>
-      <c r="F96" s="7"/>
+      <c r="A96" s="7"/>
+      <c r="B96" s="7"/>
+      <c r="C96" s="7"/>
+      <c r="D96" s="7"/>
     </row>
     <row r="97" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I97" s="7"/>
-      <c r="J97" s="7"/>
-      <c r="K97" s="7"/>
-      <c r="L97" s="7"/>
+      <c r="E97" s="7"/>
+      <c r="F97" s="7"/>
+    </row>
+    <row r="98" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="99" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I99" s="7"/>
+      <c r="J99" s="7"/>
+      <c r="K99" s="7"/>
+      <c r="L99" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Fixed issue with the npc's being distorted
</commit_message>
<xml_diff>
--- a/npc/npc.xlsx
+++ b/npc/npc.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="201">
   <si>
     <t xml:space="preserve">Scene</t>
   </si>
@@ -597,24 +597,30 @@
     <t xml:space="preserve">This is embarrassing, I’ve lost my cartography students in the walled gardens (yes I know). Please help me! Follow me to the gardens.</t>
   </si>
   <si>
+    <t xml:space="preserve">Let's Go!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scriptevent fraction:npc 0</t>
+  </si>
+  <si>
     <t xml:space="preserve">fractionNpc1</t>
   </si>
   <si>
     <t xml:space="preserve">Oh dear oh dear, please keep up I cannot lose a whole class.</t>
   </si>
   <si>
-    <t xml:space="preserve">Let's Go!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scriptevent fraction:npc 0</t>
-  </si>
-  <si>
     <t xml:space="preserve">fractionNpc2</t>
   </si>
   <si>
     <t xml:space="preserve">I need you to rescue each student that is trapped. But you CANNOT touch the grass or the groundskeeper will get very angry. Use these magical rods to reach each student. You need to work out the fractions to get to the area correctly. If you make a mistake or touch the grass head back to me to start again. You can use the numbers on the walls to work out how far each student is, and therefore which rod to use! </t>
   </si>
   <si>
+    <t xml:space="preserve">Wish me luck</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scriptevent fraction:npc 1</t>
+  </si>
+  <si>
     <t xml:space="preserve">groundskeeper</t>
   </si>
   <si>
@@ -625,12 +631,6 @@
   </si>
   <si>
     <t xml:space="preserve">tp @p 30 96 107 facing 30 96 90</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wish me luck</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scriptevent fraction:npc 1</t>
   </si>
 </sst>
 </file>
@@ -950,8 +950,8 @@
   </sheetPr>
   <dimension ref="A1:R99"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A33" colorId="64" zoomScale="109" zoomScaleNormal="109" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A61" activeCellId="0" sqref="A61"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="109" zoomScaleNormal="109" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F60" activeCellId="0" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.16796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -959,7 +959,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="82.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="114.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="38.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="18.66"/>
@@ -2138,12 +2138,16 @@
       <c r="D57" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="G57" s="3"/>
-      <c r="H57" s="4"/>
+      <c r="G57" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="H57" s="4" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>186</v>
@@ -2152,13 +2156,10 @@
         <v>187</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="H58" s="4" t="s">
-        <v>192</v>
+        <v>157</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2174,47 +2175,38 @@
       <c r="D59" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="G59" s="3" t="s">
-        <v>157</v>
+      <c r="G59" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="H59" s="4" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="G60" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="H60" s="4" t="s">
+      <c r="G60" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="H60" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G61" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="H61" s="1" t="s">
-        <v>198</v>
-      </c>
-    </row>
+    <row r="61" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="62" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C62" s="3"/>
       <c r="D62" s="5"/>
+      <c r="G62" s="3"/>
     </row>
     <row r="63" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C63" s="3"/>
@@ -2228,15 +2220,14 @@
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D65" s="5"/>
-      <c r="G65" s="3"/>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C66" s="3"/>
       <c r="D66" s="5"/>
+      <c r="G66" s="3"/>
     </row>
     <row r="67" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D67" s="6"/>
-      <c r="G67" s="3"/>
     </row>
     <row r="68" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D68" s="6"/>

</xml_diff>

<commit_message>
Changed fraction npc dialogue
</commit_message>
<xml_diff>
--- a/npc/npc.xlsx
+++ b/npc/npc.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="206">
   <si>
     <t xml:space="preserve">Scene</t>
   </si>
@@ -552,7 +552,7 @@
     <t xml:space="preserve">ratioNpc3</t>
   </si>
   <si>
-    <t xml:space="preserve">How can I help</t>
+    <t xml:space="preserve">How can I help?</t>
   </si>
   <si>
     <t xml:space="preserve">More ingredients please</t>
@@ -612,13 +612,31 @@
     <t xml:space="preserve">fractionNpc2</t>
   </si>
   <si>
-    <t xml:space="preserve">I need you to rescue each student that is trapped. But you CANNOT touch the grass or the groundskeeper will get very angry. Use these magical rods to reach each student. You need to work out the fractions to get to the area correctly. If you make a mistake or touch the grass head back to me to start again. You can use the numbers on the walls to work out how far each student is, and therefore which rod to use! </t>
+    <t xml:space="preserve">I need you to rescue each student that is trapped.  Use these magical rods to reach each student. 
+If you need to start again or get stuck come back to me!</t>
   </si>
   <si>
     <t xml:space="preserve">Wish me luck</t>
   </si>
   <si>
     <t xml:space="preserve">scriptevent fraction:npc 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fractionNpc3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start Again</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dialogue open @e[tag=fractionNpc] @p fractionNpc4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fractionNpc4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. The grids are 24x24 blocks wide and you need to use the rods to cross them.
+2. You can place the rods by right clicking in front of the white blocks. 
+3. Talk to each student as you go, they will let you know if you have placed the most optimum rod down. </t>
   </si>
   <si>
     <t xml:space="preserve">groundskeeper</t>
@@ -948,10 +966,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R99"/>
+  <dimension ref="A1:R101"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="109" zoomScaleNormal="109" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F60" activeCellId="0" sqref="F60"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="109" zoomScaleNormal="109" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D59" activeCellId="0" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.16796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2182,69 +2200,107 @@
         <v>196</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
         <v>197</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="C60" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="G60" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="D60" s="1" t="s">
+      <c r="H60" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="J60" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="G60" s="1" t="s">
+    </row>
+    <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="G61" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="H61" s="4"/>
+    </row>
+    <row r="62" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="G62" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="H60" s="1" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="62" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C62" s="3"/>
-      <c r="D62" s="5"/>
-      <c r="G62" s="3"/>
-    </row>
-    <row r="63" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C63" s="3"/>
-      <c r="D63" s="5"/>
-      <c r="G63" s="3"/>
-    </row>
+      <c r="H62" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="64" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C64" s="3"/>
       <c r="D64" s="5"/>
       <c r="G64" s="3"/>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C65" s="3"/>
       <c r="D65" s="5"/>
-    </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G65" s="3"/>
+    </row>
+    <row r="66" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C66" s="3"/>
       <c r="D66" s="5"/>
       <c r="G66" s="3"/>
     </row>
-    <row r="67" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D67" s="6"/>
-    </row>
-    <row r="68" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D68" s="6"/>
-    </row>
-    <row r="69" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D67" s="5"/>
+    </row>
+    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C68" s="3"/>
+      <c r="D68" s="5"/>
+      <c r="G68" s="3"/>
+    </row>
+    <row r="69" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D69" s="6"/>
     </row>
-    <row r="70" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D70" s="6"/>
     </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D71" s="6"/>
     </row>
-    <row r="72" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D72" s="6"/>
     </row>
-    <row r="73" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D73" s="6"/>
     </row>
     <row r="74" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2253,31 +2309,31 @@
     <row r="75" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D75" s="6"/>
     </row>
-    <row r="76" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D76" s="6"/>
     </row>
-    <row r="77" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D77" s="6"/>
     </row>
-    <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D78" s="6"/>
     </row>
     <row r="79" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D79" s="6"/>
     </row>
-    <row r="80" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D80" s="6"/>
     </row>
     <row r="81" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D81" s="6"/>
     </row>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D82" s="6"/>
     </row>
-    <row r="83" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D83" s="6"/>
     </row>
-    <row r="84" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D84" s="6"/>
     </row>
     <row r="85" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2301,30 +2357,36 @@
     <row r="91" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D91" s="6"/>
     </row>
-    <row r="92" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="93" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="94" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D94" s="6"/>
-    </row>
-    <row r="95" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D95" s="6"/>
-    </row>
+    <row r="92" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D92" s="6"/>
+    </row>
+    <row r="93" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D93" s="6"/>
+    </row>
+    <row r="94" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="95" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="96" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A96" s="7"/>
-      <c r="B96" s="7"/>
-      <c r="C96" s="7"/>
-      <c r="D96" s="7"/>
+      <c r="D96" s="6"/>
     </row>
     <row r="97" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E97" s="7"/>
-      <c r="F97" s="7"/>
-    </row>
-    <row r="98" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="D97" s="6"/>
+    </row>
+    <row r="98" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A98" s="7"/>
+      <c r="B98" s="7"/>
+      <c r="C98" s="7"/>
+      <c r="D98" s="7"/>
+    </row>
     <row r="99" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I99" s="7"/>
-      <c r="J99" s="7"/>
-      <c r="K99" s="7"/>
-      <c r="L99" s="7"/>
+      <c r="E99" s="7"/>
+      <c r="F99" s="7"/>
+    </row>
+    <row r="100" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="101" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I101" s="7"/>
+      <c r="J101" s="7"/>
+      <c r="K101" s="7"/>
+      <c r="L101" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Added the npcWalk scripts to all the npc's
</commit_message>
<xml_diff>
--- a/npc/npc.xlsx
+++ b/npc/npc.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="212">
   <si>
     <t xml:space="preserve">Scene</t>
   </si>
@@ -499,13 +499,45 @@
     <t xml:space="preserve">scaleNpc2</t>
   </si>
   <si>
-    <t xml:space="preserve">Take this stained glass and make a design using the smaller frames here. Once your design is ready, click the numerator to increase the amount the window needs to be scaled. Then right click the fraction bar to scale the window. If it fits perfectly you can move on to the next one.</t>
+    <t xml:space="preserve">Take this stained glass and make a design using the smaller frames here. 
+Once your design is ready, click the numerator to increase the amount the window needs to be scaled. 
+Then right click the fraction bar to scale the window.</t>
   </si>
   <si>
     <t xml:space="preserve">Will do</t>
   </si>
   <si>
     <t xml:space="preserve">scriptevent scale:npc 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scaleNpc3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How can I help?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">More glass please!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scriptevent scale:npc 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I’m stuck. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dialogue open @e[tag=scaleNpc] @p scaleNpc4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scaleNpc4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Place the stained glass in the frames. 
+2. Left click the numerator (top number) with the wand to change it.
+3. Right click the fraction bar to make the window appear. 
+4. If you’ve made a mistake left click the fraction bar to make it disappear.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thank you</t>
   </si>
   <si>
     <t xml:space="preserve">ratioNpc0</t>
@@ -543,25 +575,16 @@
 To make a potion mix it in the cauldron and tap it with your wand.</t>
   </si>
   <si>
-    <t xml:space="preserve">Thank you</t>
-  </si>
-  <si>
     <t xml:space="preserve">scriptevent ratio:npc 1</t>
   </si>
   <si>
     <t xml:space="preserve">ratioNpc3</t>
   </si>
   <si>
-    <t xml:space="preserve">How can I help?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">More ingredients please</t>
+    <t xml:space="preserve">More ingredients!</t>
   </si>
   <si>
     <t xml:space="preserve">scriptevent ratio:npc 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I’m stuck</t>
   </si>
   <si>
     <t xml:space="preserve">dialogue open @e[tag=ratioNpc] @p ratioNpc4</t>
@@ -966,21 +989,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R101"/>
+  <dimension ref="A1:R103"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="109" zoomScaleNormal="109" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D59" activeCellId="0" sqref="D59"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F35" colorId="64" zoomScale="109" zoomScaleNormal="109" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G56" activeCellId="0" sqref="G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.16796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="24.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="114.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="38.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="18.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="26.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="18.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="41.88"/>
@@ -2004,7 +2027,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="61.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
         <v>158</v>
       </c>
@@ -2014,7 +2037,7 @@
       <c r="C50" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="D50" s="3" t="s">
+      <c r="D50" s="5" t="s">
         <v>159</v>
       </c>
       <c r="G50" s="4" t="s">
@@ -2029,284 +2052,322 @@
         <v>162</v>
       </c>
       <c r="B51" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D51" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="G51" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="D51" s="5" t="s">
+      <c r="H51" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="G51" s="3" t="s">
+      <c r="I51" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="H51" s="4" t="s">
+      <c r="J51" s="1" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="49.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="D52" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D52" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="G52" s="3" t="s">
+      <c r="G52" s="4" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="53" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="H52" s="4"/>
+    </row>
+    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
         <v>171</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="D53" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="H53" s="4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="G53" s="3" t="s">
+      <c r="C54" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="H53" s="4" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>176</v>
+      <c r="D54" s="1" t="s">
+        <v>178</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="H54" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="I54" s="1" t="s">
         <v>179</v>
-      </c>
-      <c r="J54" s="1" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D55" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="B55" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="D55" s="5" t="s">
+      <c r="G55" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="H55" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="G55" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="H55" s="4"/>
     </row>
     <row r="56" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
         <v>183</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D56" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="D56" s="5" t="s">
+      <c r="G56" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="G56" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="H56" s="4"/>
+      <c r="H56" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="6" t="s">
-        <v>185</v>
+      <c r="A57" s="1" t="s">
+        <v>187</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
       <c r="D57" s="5" t="s">
         <v>188</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="H57" s="4" t="s">
-        <v>190</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="H57" s="4"/>
     </row>
     <row r="58" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="D58" s="6" t="s">
-        <v>192</v>
+        <v>173</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>190</v>
       </c>
       <c r="G58" s="3" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="1" t="s">
+      <c r="H58" s="4"/>
+    </row>
+    <row r="59" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C59" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>187</v>
       </c>
       <c r="D59" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="G59" s="4" t="s">
+      <c r="G59" s="3" t="s">
         <v>195</v>
       </c>
       <c r="H59" s="4" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
         <v>197</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="D60" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="G60" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D60" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="H60" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="I60" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="J60" s="1" t="s">
-        <v>199</v>
+      <c r="G60" s="3" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D61" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="B61" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="D61" s="5" t="s">
+      <c r="G61" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="G61" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="H61" s="4"/>
-    </row>
-    <row r="62" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="H61" s="4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="G62" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="H62" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="B62" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="G62" s="1" t="s">
+      <c r="I62" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="J62" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A63" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="G63" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="H63" s="4"/>
+    </row>
+    <row r="64" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A64" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="G64" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="H62" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="64" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C64" s="3"/>
-      <c r="D64" s="5"/>
-      <c r="G64" s="3"/>
-    </row>
-    <row r="65" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C65" s="3"/>
-      <c r="D65" s="5"/>
-      <c r="G65" s="3"/>
-    </row>
+      <c r="H64" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="66" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C66" s="3"/>
       <c r="D66" s="5"/>
       <c r="G66" s="3"/>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C67" s="3"/>
       <c r="D67" s="5"/>
-    </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G67" s="3"/>
+    </row>
+    <row r="68" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C68" s="3"/>
       <c r="D68" s="5"/>
       <c r="G68" s="3"/>
     </row>
-    <row r="69" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D69" s="6"/>
-    </row>
-    <row r="70" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D70" s="6"/>
-    </row>
-    <row r="71" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D69" s="5"/>
+    </row>
+    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C70" s="3"/>
+      <c r="D70" s="5"/>
+      <c r="G70" s="3"/>
+    </row>
+    <row r="71" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D71" s="6"/>
     </row>
-    <row r="72" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D72" s="6"/>
     </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D73" s="6"/>
     </row>
-    <row r="74" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D74" s="6"/>
     </row>
-    <row r="75" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D75" s="6"/>
     </row>
     <row r="76" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2315,31 +2376,31 @@
     <row r="77" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D77" s="6"/>
     </row>
-    <row r="78" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D78" s="6"/>
     </row>
-    <row r="79" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D79" s="6"/>
     </row>
-    <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D80" s="6"/>
     </row>
     <row r="81" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D81" s="6"/>
     </row>
-    <row r="82" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D82" s="6"/>
     </row>
     <row r="83" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D83" s="6"/>
     </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D84" s="6"/>
     </row>
-    <row r="85" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D85" s="6"/>
     </row>
-    <row r="86" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D86" s="6"/>
     </row>
     <row r="87" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2363,30 +2424,36 @@
     <row r="93" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D93" s="6"/>
     </row>
-    <row r="94" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="95" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="96" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D96" s="6"/>
-    </row>
-    <row r="97" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D97" s="6"/>
-    </row>
+    <row r="94" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D94" s="6"/>
+    </row>
+    <row r="95" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D95" s="6"/>
+    </row>
+    <row r="96" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="97" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="98" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A98" s="7"/>
-      <c r="B98" s="7"/>
-      <c r="C98" s="7"/>
-      <c r="D98" s="7"/>
+      <c r="D98" s="6"/>
     </row>
     <row r="99" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E99" s="7"/>
-      <c r="F99" s="7"/>
-    </row>
-    <row r="100" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="D99" s="6"/>
+    </row>
+    <row r="100" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A100" s="7"/>
+      <c r="B100" s="7"/>
+      <c r="C100" s="7"/>
+      <c r="D100" s="7"/>
+    </row>
     <row r="101" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I101" s="7"/>
-      <c r="J101" s="7"/>
-      <c r="K101" s="7"/>
-      <c r="L101" s="7"/>
+      <c r="E101" s="7"/>
+      <c r="F101" s="7"/>
+    </row>
+    <row r="102" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="103" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I103" s="7"/>
+      <c r="J103" s="7"/>
+      <c r="K103" s="7"/>
+      <c r="L103" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Added is jumping into the game
</commit_message>
<xml_diff>
--- a/npc/npc.xlsx
+++ b/npc/npc.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="214">
   <si>
     <t xml:space="preserve">Scene</t>
   </si>
@@ -672,6 +672,12 @@
   </si>
   <si>
     <t xml:space="preserve">tp @p 30 96 107 facing 30 96 90</t>
+  </si>
+  <si>
+    <t xml:space="preserve">groundskeeper1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No jumping in the gardens.</t>
   </si>
 </sst>
 </file>
@@ -681,7 +687,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -717,6 +723,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="4">
@@ -773,7 +785,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -800,6 +812,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -991,8 +1007,8 @@
   </sheetPr>
   <dimension ref="A1:R103"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F35" colorId="64" zoomScale="109" zoomScaleNormal="109" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G56" activeCellId="0" sqref="G56"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E42" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H68" activeCellId="0" sqref="H68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.16796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2331,7 +2347,26 @@
         <v>211</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="65" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A65" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="H65" s="7" t="s">
+        <v>211</v>
+      </c>
+    </row>
     <row r="66" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C66" s="3"/>
       <c r="D66" s="5"/>
@@ -2439,21 +2474,21 @@
       <c r="D99" s="6"/>
     </row>
     <row r="100" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A100" s="7"/>
-      <c r="B100" s="7"/>
-      <c r="C100" s="7"/>
-      <c r="D100" s="7"/>
+      <c r="A100" s="8"/>
+      <c r="B100" s="8"/>
+      <c r="C100" s="8"/>
+      <c r="D100" s="8"/>
     </row>
     <row r="101" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E101" s="7"/>
-      <c r="F101" s="7"/>
+      <c r="E101" s="8"/>
+      <c r="F101" s="8"/>
     </row>
     <row r="102" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="103" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I103" s="7"/>
-      <c r="J103" s="7"/>
-      <c r="K103" s="7"/>
-      <c r="L103" s="7"/>
+      <c r="I103" s="8"/>
+      <c r="J103" s="8"/>
+      <c r="K103" s="8"/>
+      <c r="L103" s="8"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Added Npc resets into the game.
</commit_message>
<xml_diff>
--- a/npc/npc.xlsx
+++ b/npc/npc.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="222">
   <si>
     <t xml:space="preserve">Scene</t>
   </si>
@@ -660,6 +660,31 @@
     <t xml:space="preserve">1. The grids are 24x24 blocks wide and you need to use the rods to cross them.
 2. You can place the rods by right clicking in front of the white blocks. 
 3. Talk to each student as you go, they will let you know if you have placed the most optimum rod down. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Well done you saved the student and made it to a checkpoint. Come back to me if you run out of rods.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">More Rods.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dialogue open @e[tag=fractionNpc] @p fractionNpc5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">farctionNpc5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Professor of Cartography </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Getting more rods will reset the game. 
+Are you sure you want to reset the game?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No thanks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reset the game. </t>
   </si>
   <si>
     <t xml:space="preserve">groundskeeper</t>
@@ -687,7 +712,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -723,12 +748,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="4">
@@ -785,7 +804,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -812,10 +831,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -1005,10 +1020,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R103"/>
+  <dimension ref="A1:R105"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E42" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H68" activeCellId="0" sqref="H68"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G58" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J65" activeCellId="0" sqref="J65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.16796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2327,88 +2342,130 @@
       </c>
       <c r="H63" s="4"/>
     </row>
-    <row r="64" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D64" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="B64" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="C64" s="1" t="s">
+      <c r="G64" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H64" s="4"/>
+      <c r="I64" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="D64" s="1" t="s">
+      <c r="J64" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="G64" s="1" t="s">
+    </row>
+    <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A65" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="G65" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="H65" s="4"/>
+      <c r="I65" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="J65" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="G66" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="H64" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A65" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="G65" s="1" t="s">
+      <c r="H66" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="G67" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="H65" s="7" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C66" s="3"/>
-      <c r="D66" s="5"/>
-      <c r="G66" s="3"/>
-    </row>
-    <row r="67" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C67" s="3"/>
-      <c r="D67" s="5"/>
-      <c r="G67" s="3"/>
+      <c r="H67" s="4" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="68" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C68" s="3"/>
       <c r="D68" s="5"/>
       <c r="G68" s="3"/>
     </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C69" s="3"/>
       <c r="D69" s="5"/>
-    </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G69" s="3"/>
+    </row>
+    <row r="70" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C70" s="3"/>
       <c r="D70" s="5"/>
       <c r="G70" s="3"/>
     </row>
-    <row r="71" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D71" s="6"/>
-    </row>
-    <row r="72" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D72" s="6"/>
-    </row>
-    <row r="73" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D71" s="5"/>
+    </row>
+    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C72" s="3"/>
+      <c r="D72" s="5"/>
+      <c r="G72" s="3"/>
+    </row>
+    <row r="73" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D73" s="6"/>
     </row>
-    <row r="74" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D74" s="6"/>
     </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D75" s="6"/>
     </row>
-    <row r="76" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D76" s="6"/>
     </row>
-    <row r="77" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D77" s="6"/>
     </row>
     <row r="78" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2417,31 +2474,31 @@
     <row r="79" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D79" s="6"/>
     </row>
-    <row r="80" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D80" s="6"/>
     </row>
-    <row r="81" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D81" s="6"/>
     </row>
-    <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D82" s="6"/>
     </row>
     <row r="83" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D83" s="6"/>
     </row>
-    <row r="84" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D84" s="6"/>
     </row>
     <row r="85" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D85" s="6"/>
     </row>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D86" s="6"/>
     </row>
-    <row r="87" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D87" s="6"/>
     </row>
-    <row r="88" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D88" s="6"/>
     </row>
     <row r="89" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2465,30 +2522,36 @@
     <row r="95" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D95" s="6"/>
     </row>
-    <row r="96" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="97" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="98" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D98" s="6"/>
-    </row>
-    <row r="99" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D99" s="6"/>
-    </row>
+    <row r="96" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D96" s="6"/>
+    </row>
+    <row r="97" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D97" s="6"/>
+    </row>
+    <row r="98" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="99" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="100" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A100" s="8"/>
-      <c r="B100" s="8"/>
-      <c r="C100" s="8"/>
-      <c r="D100" s="8"/>
+      <c r="D100" s="6"/>
     </row>
     <row r="101" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E101" s="8"/>
-      <c r="F101" s="8"/>
-    </row>
-    <row r="102" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="D101" s="6"/>
+    </row>
+    <row r="102" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A102" s="7"/>
+      <c r="B102" s="7"/>
+      <c r="C102" s="7"/>
+      <c r="D102" s="7"/>
+    </row>
     <row r="103" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I103" s="8"/>
-      <c r="J103" s="8"/>
-      <c r="K103" s="8"/>
-      <c r="L103" s="8"/>
+      <c r="E103" s="7"/>
+      <c r="F103" s="7"/>
+    </row>
+    <row r="104" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="105" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I105" s="7"/>
+      <c r="J105" s="7"/>
+      <c r="K105" s="7"/>
+      <c r="L105" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Moved the fraction npc around the map with the player
</commit_message>
<xml_diff>
--- a/npc/npc.xlsx
+++ b/npc/npc.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="224">
   <si>
     <t xml:space="preserve">Scene</t>
   </si>
@@ -648,10 +648,16 @@
     <t xml:space="preserve">fractionNpc3</t>
   </si>
   <si>
-    <t xml:space="preserve">Start Again</t>
+    <t xml:space="preserve">Help!</t>
   </si>
   <si>
     <t xml:space="preserve">dialogue open @e[tag=fractionNpc] @p fractionNpc4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start Again.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dialogue open @e[tag=fractionNpc] @p fractionNpc6</t>
   </si>
   <si>
     <t xml:space="preserve">fractionNpc4</t>
@@ -662,16 +668,16 @@
 3. Talk to each student as you go, they will let you know if you have placed the most optimum rod down. </t>
   </si>
   <si>
+    <t xml:space="preserve">fractionNpc5</t>
+  </si>
+  <si>
     <t xml:space="preserve">Well done you saved the student and made it to a checkpoint. Come back to me if you run out of rods.</t>
   </si>
   <si>
     <t xml:space="preserve">More Rods.</t>
   </si>
   <si>
-    <t xml:space="preserve">dialogue open @e[tag=fractionNpc] @p fractionNpc5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">farctionNpc5</t>
+    <t xml:space="preserve">fractionNpc6</t>
   </si>
   <si>
     <t xml:space="preserve">Professor of Cartography </t>
@@ -712,7 +718,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -748,6 +754,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="4">
@@ -804,7 +816,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -831,6 +843,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -1022,8 +1038,8 @@
   </sheetPr>
   <dimension ref="A1:R105"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G58" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J65" activeCellId="0" sqref="J65"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A65" activeCellId="0" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.16796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2314,19 +2330,19 @@
       <c r="G62" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="H62" s="4" t="s">
-        <v>202</v>
+      <c r="H62" s="7" t="s">
+        <v>205</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="J62" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
+      </c>
+      <c r="J62" s="7" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>192</v>
@@ -2335,7 +2351,7 @@
         <v>193</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="G63" s="4" t="s">
         <v>170</v>
@@ -2344,7 +2360,7 @@
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>192</v>
@@ -2353,38 +2369,38 @@
         <v>193</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="G64" s="4" t="s">
         <v>31</v>
       </c>
       <c r="H64" s="4"/>
       <c r="I64" s="1" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>192</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="G65" s="4" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="H65" s="4"/>
       <c r="I65" s="1" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="J65" s="1" t="s">
         <v>202</v>
@@ -2392,42 +2408,42 @@
     </row>
     <row r="66" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="G66" s="1" t="s">
         <v>157</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="G67" s="1" t="s">
         <v>157</v>
       </c>
       <c r="H67" s="4" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2537,21 +2553,21 @@
       <c r="D101" s="6"/>
     </row>
     <row r="102" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A102" s="7"/>
-      <c r="B102" s="7"/>
-      <c r="C102" s="7"/>
-      <c r="D102" s="7"/>
+      <c r="A102" s="8"/>
+      <c r="B102" s="8"/>
+      <c r="C102" s="8"/>
+      <c r="D102" s="8"/>
     </row>
     <row r="103" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E103" s="7"/>
-      <c r="F103" s="7"/>
+      <c r="E103" s="8"/>
+      <c r="F103" s="8"/>
     </row>
     <row r="104" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="105" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I105" s="7"/>
-      <c r="J105" s="7"/>
-      <c r="K105" s="7"/>
-      <c r="L105" s="7"/>
+      <c r="I105" s="8"/>
+      <c r="J105" s="8"/>
+      <c r="K105" s="8"/>
+      <c r="L105" s="8"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
fixed second button issue
</commit_message>
<xml_diff>
--- a/npc/npc.xlsx
+++ b/npc/npc.xlsx
@@ -376,6 +376,15 @@
     <t xml:space="preserve">Ratios</t>
   </si>
   <si>
+    <t xml:space="preserve">scriptevent spawn:npc ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scale Factors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scriptevent spawn:npc scale</t>
+  </si>
+  <si>
     <t xml:space="preserve">scaleNpc0</t>
   </si>
   <si>
@@ -427,6 +436,9 @@
   </si>
   <si>
     <t xml:space="preserve">I’m stuck. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dialogue open @e[tag=scaleNpc] @p scaleNpc4</t>
   </si>
   <si>
     <t xml:space="preserve">scaleNpc4</t>
@@ -468,15 +480,6 @@
     <t xml:space="preserve">On the way!</t>
   </si>
   <si>
-    <t xml:space="preserve">scriptevent spawn:npc ratio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scale Factors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scriptevent spawn:npc scale</t>
-  </si>
-  <si>
     <t xml:space="preserve">ratioNpc6</t>
   </si>
   <si>
@@ -498,6 +501,9 @@
   </si>
   <si>
     <t xml:space="preserve">scriptevent ratio:npc 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dialogue open @e[tag=ratioNpc] @p ratioNpc4</t>
   </si>
   <si>
     <t xml:space="preserve">ratioNpc4</t>
@@ -518,9 +524,6 @@
     <t xml:space="preserve">You broke rule number 2, you must let the potions do the work, no swimming or diving.</t>
   </si>
   <si>
-    <t xml:space="preserve">dialogue open @e[tag=scaleNpc] @p scaleNpc4</t>
-  </si>
-  <si>
     <t xml:space="preserve">ratioNpc2</t>
   </si>
   <si>
@@ -582,9 +585,6 @@
     <t xml:space="preserve">scriptevent fraction:npc 1</t>
   </si>
   <si>
-    <t xml:space="preserve">dialogue open @e[tag=ratioNpc] @p ratioNpc4</t>
-  </si>
-  <si>
     <t xml:space="preserve">fractionNpc3</t>
   </si>
   <si>
@@ -595,6 +595,9 @@
   </si>
   <si>
     <t xml:space="preserve">Start Again.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dialogue open @e[tag=fractionNpc] @p fractionNpc6</t>
   </si>
   <si>
     <t xml:space="preserve">fractionNpc4</t>
@@ -646,9 +649,6 @@
   </si>
   <si>
     <t xml:space="preserve">No jumping in the gardens.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dialogue open @e[tag=fractionNpc] @p fractionNpc6</t>
   </si>
 </sst>
 </file>
@@ -658,7 +658,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -694,18 +694,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -762,7 +750,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -789,18 +777,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -992,8 +968,8 @@
   </sheetPr>
   <dimension ref="A1:R1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C33" activeCellId="0" sqref="C33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I51" activeCellId="0" sqref="I51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.16796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1489,7 +1465,7 @@
       <c r="C23" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="6" t="s">
         <v>41</v>
       </c>
       <c r="G23" s="4" t="s">
@@ -1586,7 +1562,7 @@
       <c r="D28" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G28" s="8" t="s">
+      <c r="G28" s="4" t="s">
         <v>38</v>
       </c>
       <c r="H28" s="4"/>
@@ -1699,7 +1675,7 @@
       <c r="B34" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C34" s="9" t="s">
+      <c r="C34" s="3" t="s">
         <v>103</v>
       </c>
       <c r="D34" s="6" t="s">
@@ -1736,7 +1712,7 @@
       <c r="B36" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C36" s="9" t="s">
+      <c r="C36" s="3" t="s">
         <v>103</v>
       </c>
       <c r="D36" s="5" t="s">
@@ -1754,7 +1730,7 @@
       <c r="B37" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C37" s="9" t="s">
+      <c r="C37" s="3" t="s">
         <v>103</v>
       </c>
       <c r="D37" s="3" t="s">
@@ -1792,327 +1768,327 @@
       <c r="I38" s="4" t="s">
         <v>117</v>
       </c>
+      <c r="J38" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="K38" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="L38" s="4" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>31</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>120</v>
-      </c>
       <c r="D40" s="1" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>134</v>
+        <v>137</v>
+      </c>
+      <c r="J42" s="4" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="49.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>140</v>
-      </c>
       <c r="D45" s="1" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="J45" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="K45" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="L45" s="4" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I47" s="4" t="s">
-        <v>134</v>
+        <v>137</v>
+      </c>
+      <c r="J47" s="4" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="85.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="J49" s="4" t="s">
-        <v>161</v>
+        <v>128</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="49.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="J54" s="4" t="s">
         <v>181</v>
       </c>
     </row>
@@ -2121,13 +2097,13 @@
         <v>182</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="G55" s="4" t="s">
         <v>183</v>
@@ -2138,102 +2114,111 @@
       <c r="I55" s="4" t="s">
         <v>185</v>
       </c>
+      <c r="J55" s="4" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="G57" s="4" t="s">
         <v>31</v>
       </c>
       <c r="I57" s="4" t="s">
-        <v>190</v>
+        <v>191</v>
+      </c>
+      <c r="J57" s="4" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I58" s="4" t="s">
-        <v>195</v>
+        <v>196</v>
+      </c>
+      <c r="J58" s="4" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="H60" s="1" t="s">
         <v>200</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="G60" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="H60" s="1" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2245,9 +2230,6 @@
       <c r="C62" s="3"/>
       <c r="D62" s="5"/>
       <c r="G62" s="3"/>
-      <c r="J62" s="4" t="s">
-        <v>202</v>
-      </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C63" s="3"/>
@@ -2256,17 +2238,11 @@
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D64" s="5"/>
-      <c r="J64" s="4" t="s">
-        <v>202</v>
-      </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C65" s="3"/>
       <c r="D65" s="5"/>
       <c r="G65" s="3"/>
-      <c r="J65" s="4" t="s">
-        <v>180</v>
-      </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D66" s="6"/>
@@ -2352,18 +2328,18 @@
       <c r="D94" s="6"/>
     </row>
     <row r="95" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A95" s="10"/>
-      <c r="B95" s="10"/>
-      <c r="C95" s="10"/>
-      <c r="D95" s="10"/>
+      <c r="A95" s="7"/>
+      <c r="B95" s="7"/>
+      <c r="C95" s="7"/>
+      <c r="D95" s="7"/>
     </row>
     <row r="96" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E96" s="10"/>
-      <c r="F96" s="10"/>
+      <c r="E96" s="7"/>
+      <c r="F96" s="7"/>
     </row>
     <row r="97" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="98" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I98" s="10"/>
+      <c r="I98" s="7"/>
     </row>
     <row r="99" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="100" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2372,9 +2348,9 @@
     <row r="103" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="104" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="105" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J105" s="10"/>
-      <c r="K105" s="10"/>
-      <c r="L105" s="10"/>
+      <c r="J105" s="7"/>
+      <c r="K105" s="7"/>
+      <c r="L105" s="7"/>
     </row>
     <row r="106" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="107" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Rod game mostly stable
</commit_message>
<xml_diff>
--- a/npc/npc.xlsx
+++ b/npc/npc.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="204">
   <si>
     <t xml:space="preserve">Scene</t>
   </si>
@@ -331,7 +331,7 @@
     <t xml:space="preserve">rodNpc8</t>
   </si>
   <si>
-    <t xml:space="preserve">Groundskeeper</t>
+    <t xml:space="preserve">Isabella</t>
   </si>
   <si>
     <t xml:space="preserve">You’ve completed the game and saved all the students. Great work.</t>
@@ -343,13 +343,16 @@
     <t xml:space="preserve">rodNpc8Fail</t>
   </si>
   <si>
+    <t xml:space="preserve">ERROR  It means the rods quantities are wrong. </t>
+  </si>
+  <si>
     <t xml:space="preserve">scriptevent rod:npcReplay 8</t>
   </si>
   <si>
     <t xml:space="preserve">rodNpc8Saved</t>
   </si>
   <si>
-    <t xml:space="preserve">Thanks for rescuing me, wait I didn’t need rescuing!!!</t>
+    <t xml:space="preserve">Thanks for rescuing me, I’m the last one. </t>
   </si>
   <si>
     <t xml:space="preserve">Okay ..</t>
@@ -699,7 +702,7 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="0"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -978,8 +981,8 @@
   </sheetPr>
   <dimension ref="A1:R1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D7" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H37" activeCellId="0" sqref="H37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D36" activeCellId="0" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.16796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -987,7 +990,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="24.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="129.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="143.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="38.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="27"/>
@@ -1538,7 +1541,7 @@
       <c r="G26" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="H26" s="7" t="s">
+      <c r="H26" s="4" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1558,7 +1561,7 @@
       <c r="G27" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H27" s="7" t="s">
+      <c r="H27" s="4" t="s">
         <v>89</v>
       </c>
       <c r="I27" s="4" t="s">
@@ -1599,8 +1602,6 @@
       <c r="G29" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H29" s="0"/>
-      <c r="I29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
@@ -1679,8 +1680,6 @@
       <c r="G33" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H33" s="0"/>
-      <c r="I33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
@@ -1709,17 +1708,17 @@
       <c r="B35" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="7" t="s">
         <v>103</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>41</v>
+        <v>107</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>26</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I35" s="4" t="s">
         <v>28</v>
@@ -1727,30 +1726,30 @@
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="7" t="s">
         <v>103</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H36" s="4"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="7" t="s">
         <v>103</v>
       </c>
       <c r="D37" s="3" t="s">
@@ -1759,482 +1758,480 @@
       <c r="G37" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H37" s="0"/>
-      <c r="I37" s="0"/>
     </row>
     <row r="38" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="L38" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>31</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="49.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="I47" s="4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="85.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="49.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="6" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="H55" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="I55" s="4" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="G57" s="4" t="s">
         <v>31</v>
       </c>
       <c r="I57" s="4" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="I58" s="4" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="J58" s="4" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="H60" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="G60" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="H60" s="1" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Checkpoints added to the game.
</commit_message>
<xml_diff>
--- a/npc/npc.xlsx
+++ b/npc/npc.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="205">
   <si>
     <t xml:space="preserve">Scene</t>
   </si>
@@ -97,16 +97,16 @@
     <t xml:space="preserve">rodNpc0Fail</t>
   </si>
   <si>
-    <t xml:space="preserve">You saved me! However, you made up a half out of multiple fractions. I can show you a more optimum way. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Show me </t>
+    <t xml:space="preserve">You saved me! If you want to get more students I can show you how to use the rods more efficiently.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show me.</t>
   </si>
   <si>
     <t xml:space="preserve">scriptevent rod:npcReplay 0</t>
   </si>
   <si>
-    <t xml:space="preserve">Not Interested!</t>
+    <t xml:space="preserve">I’ll carry on.</t>
   </si>
   <si>
     <t xml:space="preserve">rodNpc0Default</t>
@@ -115,289 +115,292 @@
     <t xml:space="preserve">Help me! You can only rescue me if you use the right amount of rods to get to this platform, otherwise I can't get back safely. If you need to start again talk to the Prof.</t>
   </si>
   <si>
+    <t xml:space="preserve">Okay.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc0Saved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thanks for rescuing me!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc1Win</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lisa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You saved me! 12 is half of 24 and you used the right rod to get here.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You’re Welcome.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scriptevent rod:npcComplete 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc1Fail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show me .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scriptevent rod:npcReplay 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc1Default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc1Saved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc2Win</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Callum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You saved me! 4 is a sixth of 24 and you used the right rod to get here.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scriptevent rod:npcComplete 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc2Fail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scriptevent rod:npcReplay 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc2Default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc2Saved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc3Win</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deena</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Great work you made ¾ in the most optimum way by combining  ½ and ¼ .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scriptevent rod:npcComplete 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc3Fail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scriptevent rod:npcReplay 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc3Default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc3Saved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc4Win</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Well done! You combined ¼ with 1/8 to make 3/8.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Great.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scriptevent rod:npcComplete 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc4Fail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scriptevent rod:npcReplay 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc4Default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc4Saved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc5Win</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isaac</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wow, great working going over 1 tweed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scriptevent rod:npcComplete 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc5Fail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scriptevent rod:npcReplay 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc5Default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc5Saved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc6Win</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tamsin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Well done, 3/1 is 36, great work.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thanks.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scriptevent rod:npcComplete 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc6Fail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scriptevent rod:npcReplay 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc6Saved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc6Default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc7Win</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fleur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You saved me! 3 is indeed 1/8 of 24, you used the right rod.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scriptevent rod:npcComplete 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc7Fail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scriptevent rod:npcReplay 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc7Saved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc7Default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc8Win</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isabella</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You’ve completed the game and saved all the students. Great work.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scriptevent rod:npcComplete 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc8Fail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERROR This shouldn’t appear in the game.  It means the rods quantities are wrong. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">scriptevent rod:npcReplay 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc8Saved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thanks for rescuing me, I’m the last one. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Okay .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rodNpc8Default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spawnNpc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dean of Students</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Welcome! We need your help with three different maths challenges. Pick one below, then a Professor from that school will guide you from the courtyard ahead.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fractions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scriptevent spawn:npc fraction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ratios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scriptevent spawn:npc ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scale Factors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scriptevent spawn:npc scale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scaleNpc0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scaleNpc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guild Master</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This old building desperately needs some new windows. The architecture team needs the help of a Mathmogician to scale it correctly. Follow me!</t>
+  </si>
+  <si>
     <t xml:space="preserve">Okay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc0Saved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thanks for rescuing me!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc1Win</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lisa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You saved me! 12 is half of 24 and you used the right rod to get here.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You’re Welcome</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scriptevent rod:npcComplete 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc1Fail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Well done, you made it! But there is a more optimum route to get here, can I show you?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scriptevent rod:npcReplay 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc1Default</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc1Saved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc2Win</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Callum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You saved me! 4 is a sixth of 24 and you used the right rod to get here.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scriptevent rod:npcComplete 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc2Fail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scriptevent rod:npcReplay 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc2Default</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc2Saved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc3Win</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deena</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Great work you made ¾ in the most optimum way by combining  ½ and ¼ .</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scriptevent rod:npcComplete 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc3Fail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scriptevent rod:npcReplay 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc3Default</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc3Saved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc4Win</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eli</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Well done! You combined ¼ with 1/8 to make 3/8.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Great</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scriptevent rod:npcComplete 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc4Fail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scriptevent rod:npcReplay 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc4Default</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc4Saved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc5Win</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Isaac</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wow, great working going over 1 tweed.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scriptevent rod:npcComplete 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc5Fail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scriptevent rod:npcReplay 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc5Default</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc5Saved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc6Win</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tamsin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Well done, 3/1 is 36, great work.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thanks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scriptevent rod:npcComplete 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc6Fail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scriptevent rod:npcReplay 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc6Saved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc6Default</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc7Win</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fleur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You saved me! 3 is indeed 1/8 of 24, you used the right rod.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scriptevent rod:npcComplete 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc7Fail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scriptevent rod:npcReplay 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc7Saved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc7Default</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc8Win</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Isabella</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You’ve completed the game and saved all the students. Great work.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scriptevent rod:npcComplete 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc8Fail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ERROR  It means the rods quantities are wrong. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">scriptevent rod:npcReplay 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc8Saved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thanks for rescuing me, I’m the last one. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Okay ..</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rodNpc8Default</t>
-  </si>
-  <si>
-    <t xml:space="preserve">spawnNpc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dean of Students</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Welcome! We need your help with three different maths challenges. Pick one below, then a Professor from that school will guide you from the courtyard ahead.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fractions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scriptevent spawn:npc fraction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ratios</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scriptevent spawn:npc ratio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scale Factors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scriptevent spawn:npc scale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scaleNpc0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scaleNpc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Guild Master</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This old building desperately needs some new windows. The architecture team needs the help of a Mathmogician to scale it correctly. Follow me!</t>
   </si>
   <si>
     <t xml:space="preserve">scriptevent scale:npc 0</t>
@@ -606,7 +609,7 @@
     <t xml:space="preserve">fractionNpc4</t>
   </si>
   <si>
-    <t xml:space="preserve">1. The grids are 24x24 blocks wide and you need to use the rods to cross them.
+    <t xml:space="preserve">1. There are three grids two are  24x24 blocks wide and one is 48 x24 you need to use the rods to cross them.
 2. You can place the rods by right clicking in front of the white blocks. 
 3. Talk to each student as you go, they will let you know if you have placed the most optimum rod down. </t>
   </si>
@@ -645,7 +648,7 @@
     <t xml:space="preserve">Grrrrofffff me grass</t>
   </si>
   <si>
-    <t xml:space="preserve">tp @p 30 96 107 facing 30 96 90</t>
+    <t xml:space="preserve">scriptevent fraction:groundskeeper 0</t>
   </si>
   <si>
     <t xml:space="preserve">groundskeeper1</t>
@@ -702,7 +705,7 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="4">
@@ -780,16 +783,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -981,8 +984,8 @@
   </sheetPr>
   <dimension ref="A1:R1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D36" activeCellId="0" sqref="D36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.16796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1105,6 +1108,9 @@
       <c r="I3" s="4" t="s">
         <v>28</v>
       </c>
+      <c r="J3" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -1171,16 +1177,19 @@
         <v>36</v>
       </c>
       <c r="D7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>26</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="I7" s="5" t="s">
         <v>28</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1227,7 +1236,7 @@
       <c r="C10" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="6" t="s">
         <v>48</v>
       </c>
       <c r="G10" s="4" t="s">
@@ -1248,16 +1257,19 @@
         <v>47</v>
       </c>
       <c r="D11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>26</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="I11" s="5" t="s">
         <v>28</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1304,7 +1316,7 @@
       <c r="C14" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="6" t="s">
         <v>57</v>
       </c>
       <c r="G14" s="4" t="s">
@@ -1324,17 +1336,20 @@
       <c r="C15" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>26</v>
       </c>
       <c r="H15" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="I15" s="5" t="s">
         <v>28</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1381,7 +1396,7 @@
       <c r="C18" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="6" t="s">
         <v>66</v>
       </c>
       <c r="G18" s="3" t="s">
@@ -1402,16 +1417,19 @@
         <v>65</v>
       </c>
       <c r="D19" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G19" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>26</v>
       </c>
       <c r="H19" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="I19" s="4" t="s">
+      <c r="I19" s="5" t="s">
         <v>28</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1458,7 +1476,7 @@
       <c r="C22" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="7" t="s">
         <v>76</v>
       </c>
       <c r="G22" s="4" t="s">
@@ -1479,16 +1497,19 @@
         <v>75</v>
       </c>
       <c r="D23" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G23" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>26</v>
       </c>
       <c r="H23" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="I23" s="4" t="s">
+      <c r="I23" s="5" t="s">
         <v>28</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1535,7 +1556,7 @@
       <c r="C26" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="6" t="s">
         <v>85</v>
       </c>
       <c r="G26" s="3" t="s">
@@ -1556,16 +1577,19 @@
         <v>84</v>
       </c>
       <c r="D27" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G27" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>26</v>
       </c>
       <c r="H27" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="I27" s="4" t="s">
+      <c r="I27" s="5" t="s">
         <v>28</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1578,7 +1602,7 @@
       <c r="C28" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="D28" s="7" t="s">
         <v>33</v>
       </c>
       <c r="G28" s="4" t="s">
@@ -1613,7 +1637,7 @@
       <c r="C30" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D30" s="6" t="s">
         <v>95</v>
       </c>
       <c r="G30" s="4" t="s">
@@ -1633,17 +1657,20 @@
       <c r="C31" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D31" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G31" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>26</v>
       </c>
       <c r="H31" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="I31" s="4" t="s">
+      <c r="I31" s="5" t="s">
         <v>28</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1656,7 +1683,7 @@
       <c r="C32" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="6" t="s">
         <v>33</v>
       </c>
       <c r="G32" s="4" t="s">
@@ -1691,7 +1718,7 @@
       <c r="C34" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="D34" s="7" t="s">
         <v>104</v>
       </c>
       <c r="G34" s="4" t="s">
@@ -1708,20 +1735,23 @@
       <c r="B35" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="C35" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D35" s="6" t="s">
         <v>107</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="H35" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="I35" s="4" t="s">
+      <c r="I35" s="5" t="s">
         <v>28</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1731,10 +1761,10 @@
       <c r="B36" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="C36" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D36" s="6" t="s">
         <v>110</v>
       </c>
       <c r="G36" s="4" t="s">
@@ -1749,7 +1779,7 @@
       <c r="B37" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="C37" s="3" t="s">
         <v>103</v>
       </c>
       <c r="D37" s="3" t="s">
@@ -1769,7 +1799,7 @@
       <c r="C38" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="D38" s="6" t="s">
         <v>115</v>
       </c>
       <c r="G38" s="4" t="s">
@@ -1801,19 +1831,19 @@
       <c r="C39" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="D39" s="6" t="s">
         <v>125</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>31</v>
+        <v>126</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>123</v>
@@ -1822,15 +1852,15 @@
         <v>124</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>123</v>
@@ -1838,19 +1868,19 @@
       <c r="C41" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="D41" s="5" t="s">
-        <v>131</v>
+      <c r="D41" s="6" t="s">
+        <v>132</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>123</v>
@@ -1859,24 +1889,24 @@
         <v>124</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="49.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>123</v>
@@ -1884,461 +1914,461 @@
       <c r="C43" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="D43" s="5" t="s">
-        <v>141</v>
+      <c r="D43" s="6" t="s">
+        <v>142</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D44" s="5" t="s">
         <v>146</v>
       </c>
+      <c r="D44" s="6" t="s">
+        <v>147</v>
+      </c>
       <c r="G44" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>153</v>
+        <v>146</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>154</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>135</v>
+        <v>146</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>136</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="I47" s="4" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="85.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>161</v>
+        <v>146</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>162</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>163</v>
+        <v>146</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>164</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>165</v>
+        <v>146</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>166</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="49.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>169</v>
+        <v>146</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>170</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="6" t="s">
-        <v>171</v>
+      <c r="A52" s="7" t="s">
+        <v>172</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="D52" s="5" t="s">
         <v>174</v>
       </c>
+      <c r="D52" s="6" t="s">
+        <v>175</v>
+      </c>
       <c r="G52" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D53" s="6" t="s">
-        <v>178</v>
+        <v>174</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>179</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>180</v>
+        <v>174</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>181</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>135</v>
+        <v>174</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>136</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H55" s="4" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="I55" s="4" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>189</v>
+        <v>174</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>190</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>191</v>
+        <v>174</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>192</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>31</v>
+        <v>126</v>
       </c>
       <c r="I57" s="4" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="D58" s="5" t="s">
         <v>195</v>
       </c>
+      <c r="D58" s="6" t="s">
+        <v>196</v>
+      </c>
       <c r="G58" s="4" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="I58" s="4" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="J58" s="4" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H60" s="4" t="s">
         <v>202</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="G60" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="H60" s="1" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C61" s="3"/>
-      <c r="D61" s="5"/>
+      <c r="D61" s="6"/>
       <c r="G61" s="3"/>
     </row>
     <row r="62" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C62" s="3"/>
-      <c r="D62" s="5"/>
+      <c r="D62" s="6"/>
       <c r="G62" s="3"/>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C63" s="3"/>
-      <c r="D63" s="5"/>
+      <c r="D63" s="6"/>
       <c r="G63" s="3"/>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D64" s="5"/>
+      <c r="D64" s="6"/>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C65" s="3"/>
-      <c r="D65" s="5"/>
+      <c r="D65" s="6"/>
       <c r="G65" s="3"/>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D66" s="6"/>
+      <c r="D66" s="7"/>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D67" s="6"/>
+      <c r="D67" s="7"/>
     </row>
     <row r="68" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D68" s="6"/>
+      <c r="D68" s="7"/>
     </row>
     <row r="69" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D69" s="6"/>
+      <c r="D69" s="7"/>
     </row>
     <row r="70" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D70" s="6"/>
+      <c r="D70" s="7"/>
     </row>
     <row r="71" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D71" s="6"/>
+      <c r="D71" s="7"/>
     </row>
     <row r="72" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D72" s="6"/>
+      <c r="D72" s="7"/>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D73" s="6"/>
+      <c r="D73" s="7"/>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D74" s="6"/>
+      <c r="D74" s="7"/>
     </row>
     <row r="75" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D75" s="6"/>
+      <c r="D75" s="7"/>
     </row>
     <row r="76" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D76" s="6"/>
+      <c r="D76" s="7"/>
     </row>
     <row r="77" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D77" s="6"/>
+      <c r="D77" s="7"/>
     </row>
     <row r="78" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D78" s="6"/>
+      <c r="D78" s="7"/>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D79" s="6"/>
+      <c r="D79" s="7"/>
     </row>
     <row r="80" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D80" s="6"/>
+      <c r="D80" s="7"/>
     </row>
     <row r="81" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D81" s="6"/>
+      <c r="D81" s="7"/>
     </row>
     <row r="82" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D82" s="6"/>
+      <c r="D82" s="7"/>
     </row>
     <row r="83" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D83" s="6"/>
+      <c r="D83" s="7"/>
     </row>
     <row r="84" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D84" s="6"/>
+      <c r="D84" s="7"/>
     </row>
     <row r="85" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D85" s="6"/>
+      <c r="D85" s="7"/>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D86" s="6"/>
+      <c r="D86" s="7"/>
     </row>
     <row r="87" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D87" s="6"/>
+      <c r="D87" s="7"/>
     </row>
     <row r="88" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D88" s="6"/>
+      <c r="D88" s="7"/>
     </row>
     <row r="89" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D89" s="6"/>
+      <c r="D89" s="7"/>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D90" s="6"/>
+      <c r="D90" s="7"/>
     </row>
     <row r="91" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="92" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="93" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D93" s="6"/>
+      <c r="D93" s="7"/>
     </row>
     <row r="94" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D94" s="6"/>
+      <c r="D94" s="7"/>
     </row>
     <row r="95" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="8"/>

</xml_diff>

<commit_message>
Rod game is complete
</commit_message>
<xml_diff>
--- a/npc/npc.xlsx
+++ b/npc/npc.xlsx
@@ -975,10 +975,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R1048576"/>
+  <dimension ref="A1:R107"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F46" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J58" activeCellId="0" sqref="J58"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H59" activeCellId="0" sqref="H59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.16796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2390,8 +2390,6 @@
     </row>
     <row r="106" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="107" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Added start of npc dialogue in
</commit_message>
<xml_diff>
--- a/npc/npc.xlsx
+++ b/npc/npc.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="216">
   <si>
     <t xml:space="preserve">Scene</t>
   </si>
@@ -418,9 +418,9 @@
     <t xml:space="preserve">scaleNpc2</t>
   </si>
   <si>
-    <t xml:space="preserve">Take this stained glass and make a design using the smaller frames here. 
-Once your design is ready, click the numerator to increase the amount the window needs to be scaled. 
-Then right click the fraction bar to scale the window.</t>
+    <t xml:space="preserve">The design has already been done, but I need your help to scale it. 
+Click on the numerator (top number) to change the scale size. You can count the number of blocks in the frame to work it out. 
+Then click on the orb of scaling to my right, to scale the window.</t>
   </si>
   <si>
     <t xml:space="preserve">Will do</t>
@@ -457,6 +457,36 @@
   </si>
   <si>
     <t xml:space="preserve">Thank you</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scaleNpc5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GuildMaster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">That window fits beautifully! Do you want to keep it and move on or redesign it?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carry on.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scriptevent scale:npc 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Redesign it.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scriptevent scale:npc 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scaleNpc6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oh my goodness, that’s too big! Try again. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ScaleNpc 7</t>
   </si>
   <si>
     <t xml:space="preserve">ratioNpc0</t>
@@ -977,8 +1007,8 @@
   </sheetPr>
   <dimension ref="A1:R107"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H59" activeCellId="0" sqref="H59"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C16" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D41" activeCellId="0" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.16796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1915,74 +1945,85 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1" t="s">
+      <c r="A44" s="0" t="s">
         <v>144</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="C44" s="0" t="s">
         <v>145</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="D44" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="D44" s="5" t="s">
+      <c r="E44" s="0"/>
+      <c r="F44" s="0"/>
+      <c r="G44" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="G44" s="3" t="s">
+      <c r="H44" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="H44" s="4" t="s">
+      <c r="I44" s="0" t="s">
         <v>149</v>
       </c>
+      <c r="J44" s="0" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="B45" s="1" t="s">
+      <c r="A45" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="C45" s="0" t="s">
         <v>145</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="G45" s="3" t="s">
+      <c r="D45" s="0" t="s">
         <v>152</v>
       </c>
+      <c r="E45" s="0"/>
+      <c r="F45" s="0"/>
+      <c r="G45" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="H45" s="0"/>
+      <c r="I45" s="0"/>
+      <c r="J45" s="0"/>
     </row>
     <row r="46" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1" t="s">
+      <c r="A46" s="0" t="s">
         <v>153</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="C46" s="0" t="s">
         <v>145</v>
       </c>
-      <c r="C46" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="G46" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="H46" s="4" t="s">
-        <v>156</v>
-      </c>
+      <c r="D46" s="0"/>
+      <c r="E46" s="0"/>
+      <c r="F46" s="0"/>
+      <c r="G46" s="0"/>
+      <c r="H46" s="0"/>
+      <c r="I46" s="0"/>
+      <c r="J46" s="0"/>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D47" s="5" t="s">
         <v>157</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>136</v>
       </c>
       <c r="G47" s="3" t="s">
         <v>158</v>
@@ -1990,28 +2031,22 @@
       <c r="H47" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="I47" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="J47" s="4" t="s">
+    </row>
+    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="48" customFormat="false" ht="85.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="s">
+      <c r="B48" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D48" s="5" t="s">
+      <c r="G48" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="G48" s="3" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2019,179 +2054,176 @@
         <v>163</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="D49" s="5" t="s">
         <v>164</v>
       </c>
       <c r="G49" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="H49" s="4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="I50" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="J50" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="85.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="G52" s="3" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="G50" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="H50" s="4" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="49.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="G51" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="H51" s="4" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="D52" s="5" t="s">
+    <row r="53" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="G52" s="3" t="s">
+      <c r="B53" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D53" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="H52" s="4" t="s">
+      <c r="G53" s="3" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="1" t="s">
+      <c r="H53" s="4" t="s">
         <v>178</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="D53" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="G53" s="3" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D54" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="D54" s="5" t="s">
+      <c r="G54" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="H54" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="G54" s="4" t="s">
+    </row>
+    <row r="55" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="H54" s="4" t="s">
+      <c r="B55" s="4" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="55" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="1" t="s">
+      <c r="C55" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="B55" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>174</v>
-      </c>
       <c r="D55" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="G55" s="4" t="s">
         <v>185</v>
       </c>
+      <c r="G55" s="3" t="s">
+        <v>186</v>
+      </c>
       <c r="H55" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="I55" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="J55" s="4" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D56" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="G56" s="4" t="s">
-        <v>143</v>
+      <c r="G56" s="3" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D57" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="B57" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="D57" s="5" t="s">
+      <c r="G57" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="G57" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="I57" s="4" t="s">
+      <c r="H57" s="4" t="s">
         <v>193</v>
-      </c>
-      <c r="J57" s="4" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2199,78 +2231,129 @@
         <v>194</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
       <c r="C58" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="G58" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="D58" s="5" t="s">
+      <c r="H58" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="G58" s="4" t="s">
+      <c r="I58" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="I58" s="4" t="s">
+      <c r="J58" s="4" t="s">
         <v>198</v>
-      </c>
-      <c r="J58" s="4" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D59" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="B59" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="G59" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="H59" s="1" t="s">
-        <v>203</v>
+      <c r="G59" s="4" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="G60" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="I60" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="J60" s="4" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="D60" s="1" t="s">
+      <c r="B61" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C61" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="G60" s="1" t="s">
+      <c r="D61" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="G61" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="I61" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="J61" s="4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="G62" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="H60" s="4" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C61" s="3"/>
-      <c r="D61" s="5"/>
-      <c r="G61" s="3"/>
-    </row>
-    <row r="62" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C62" s="3"/>
-      <c r="D62" s="5"/>
-      <c r="G62" s="3"/>
+      <c r="H62" s="1" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C63" s="3"/>
-      <c r="D63" s="5"/>
-      <c r="G63" s="3"/>
+      <c r="A63" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H63" s="4" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D64" s="5"/>

</xml_diff>

<commit_message>
first 3 windows working
</commit_message>
<xml_diff>
--- a/npc/npc.xlsx
+++ b/npc/npc.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="229">
   <si>
     <t xml:space="preserve">Scene</t>
   </si>
@@ -462,9 +462,6 @@
     <t xml:space="preserve">scaleNpc5</t>
   </si>
   <si>
-    <t xml:space="preserve">GuildMaster</t>
-  </si>
-  <si>
     <t xml:space="preserve">That window fits beautifully! Do you want to keep it and move on or redesign it?</t>
   </si>
   <si>
@@ -486,7 +483,49 @@
     <t xml:space="preserve">Oh my goodness, that’s too big! Try again. </t>
   </si>
   <si>
-    <t xml:space="preserve">ScaleNpc 7</t>
+    <t xml:space="preserve">scaleNpc7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I need it to fill the frame. Make it bigger.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scaleNpc8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Impressive work, if you are finished let’s take a tour of what you have created. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Let’s Go.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scriptevent scale:npc 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scaleNpc9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You’ve done really well to reach this point. The next challenges are much harder so you can graduate now if you want. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">scriptevent scale:npc6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Graduate.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scriptevent scale:npc7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scaleNpc10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You are true artisan, it’s time to graduate with full honours.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Graduate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scriptevent scale:npc8</t>
   </si>
   <si>
     <t xml:space="preserve">ratioNpc0</t>
@@ -735,7 +774,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -746,12 +785,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF44546A"/>
         <bgColor rgb="FF333399"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
       </patternFill>
     </fill>
   </fills>
@@ -789,7 +822,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -816,10 +849,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1007,8 +1036,8 @@
   </sheetPr>
   <dimension ref="A1:R107"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C16" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D41" activeCellId="0" sqref="D41"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I47" activeCellId="0" sqref="I47:J47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.16796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1945,107 +1974,109 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+      <c r="A44" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B44" s="0" t="s">
+      <c r="B44" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C44" s="0" t="s">
+      <c r="C44" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D44" s="0" t="s">
+      <c r="G44" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E44" s="0"/>
-      <c r="F44" s="0"/>
-      <c r="G44" s="0" t="s">
+      <c r="H44" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="H44" s="0" t="s">
+      <c r="I44" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="I44" s="0" t="s">
+      <c r="J44" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="J44" s="0" t="s">
+    </row>
+    <row r="45" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="45" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+      <c r="B45" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B45" s="0" t="s">
+      <c r="G45" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C45" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="D45" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="E45" s="0"/>
-      <c r="F45" s="0"/>
-      <c r="G45" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="H45" s="0"/>
-      <c r="I45" s="0"/>
-      <c r="J45" s="0"/>
-    </row>
-    <row r="46" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+      <c r="C46" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B46" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="C46" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="D46" s="0"/>
-      <c r="E46" s="0"/>
-      <c r="F46" s="0"/>
-      <c r="G46" s="0"/>
-      <c r="H46" s="0"/>
-      <c r="I46" s="0"/>
-      <c r="J46" s="0"/>
+      <c r="G46" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
         <v>154</v>
       </c>
       <c r="B47" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="G47" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D47" s="5" t="s">
+      <c r="H47" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="G47" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="H47" s="4" t="s">
-        <v>159</v>
-      </c>
+      <c r="J47" s="4"/>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H48" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D48" s="1" t="s">
+      <c r="I48" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="G48" s="3" t="s">
+      <c r="J48" s="1" t="s">
         <v>162</v>
       </c>
     </row>
@@ -2054,18 +2085,18 @@
         <v>163</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>155</v>
+        <v>123</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D49" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="G49" s="3" t="s">
+      <c r="G49" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="H49" s="4" t="s">
+      <c r="H49" s="1" t="s">
         <v>166</v>
       </c>
     </row>
@@ -2074,119 +2105,116 @@
         <v>167</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>155</v>
+        <v>168</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>156</v>
+        <v>169</v>
       </c>
       <c r="D50" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="61.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="H52" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D53" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="G50" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="H50" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="I50" s="4" t="s">
+      <c r="G53" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="H53" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="I53" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="J50" s="4" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="85.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="G51" s="3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="G52" s="3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="G53" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="H53" s="4" t="s">
-        <v>178</v>
+      <c r="J53" s="4" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>155</v>
+        <v>168</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>156</v>
+        <v>169</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="H54" s="4" t="s">
-        <v>181</v>
+        <v>143</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>184</v>
+      <c r="A55" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>169</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="H55" s="4" t="s">
-        <v>187</v>
+        <v>130</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2194,145 +2222,139 @@
         <v>188</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D56" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="D56" s="5" t="s">
         <v>189</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>130</v>
+        <v>190</v>
+      </c>
+      <c r="H56" s="4" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="G57" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="B57" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="G57" s="4" t="s">
-        <v>192</v>
-      </c>
       <c r="H57" s="4" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>184</v>
+      <c r="A58" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>197</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="G58" s="4" t="s">
-        <v>195</v>
+        <v>198</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>199</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="I58" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="J58" s="4" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>183</v>
+        <v>196</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="G59" s="4" t="s">
-        <v>143</v>
+        <v>197</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>183</v>
+        <v>196</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>184</v>
+        <v>197</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="I60" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="J60" s="4" t="s">
-        <v>198</v>
+        <v>205</v>
+      </c>
+      <c r="H60" s="4" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>183</v>
+        <v>196</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>206</v>
+        <v>136</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>207</v>
+        <v>208</v>
+      </c>
+      <c r="H61" s="4" t="s">
+        <v>209</v>
       </c>
       <c r="I61" s="4" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="J61" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="G62" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="H62" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D62" s="5" t="s">
         <v>213</v>
+      </c>
+      <c r="G62" s="4" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2340,34 +2362,89 @@
         <v>214</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
       <c r="C63" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="G63" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="I63" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="J63" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="D63" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="G63" s="1" t="s">
+    </row>
+    <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A64" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="G64" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="I64" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="J64" s="4" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A65" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="G65" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="H63" s="4" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D64" s="5"/>
-    </row>
-    <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C65" s="3"/>
-      <c r="D65" s="5"/>
-      <c r="G65" s="3"/>
+      <c r="H65" s="1" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D66" s="6"/>
+      <c r="A66" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H66" s="4" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D67" s="6"/>
+      <c r="D67" s="5"/>
     </row>
     <row r="68" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D68" s="6"/>
@@ -2443,34 +2520,18 @@
     <row r="93" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D93" s="6"/>
     </row>
-    <row r="94" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D94" s="6"/>
-    </row>
-    <row r="95" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A95" s="7"/>
-      <c r="B95" s="7"/>
-      <c r="C95" s="7"/>
-      <c r="D95" s="7"/>
-    </row>
-    <row r="96" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E96" s="7"/>
-      <c r="F96" s="7"/>
-    </row>
+    <row r="94" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="95" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="96" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="97" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="98" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I98" s="7"/>
-    </row>
+    <row r="98" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="99" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="100" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="101" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="102" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="103" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="104" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="105" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="J105" s="7"/>
-      <c r="K105" s="7"/>
-      <c r="L105" s="7"/>
-    </row>
+    <row r="105" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="106" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="107" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>

<commit_message>
reset the game sorted
</commit_message>
<xml_diff>
--- a/npc/npc.xlsx
+++ b/npc/npc.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="227">
   <si>
     <t xml:space="preserve">Scene</t>
   </si>
@@ -507,13 +507,10 @@
     <t xml:space="preserve">You’ve done really well to reach this point. The next challenges are much harder so you can graduate now if you want. </t>
   </si>
   <si>
-    <t xml:space="preserve">scriptevent scale:npc6</t>
-  </si>
-  <si>
     <t xml:space="preserve">Graduate.</t>
   </si>
   <si>
-    <t xml:space="preserve">scriptevent scale:npc7</t>
+    <t xml:space="preserve">scriptevent scale:npc 6</t>
   </si>
   <si>
     <t xml:space="preserve">scaleNpc10</t>
@@ -523,9 +520,6 @@
   </si>
   <si>
     <t xml:space="preserve">Graduate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scriptevent scale:npc8</t>
   </si>
   <si>
     <t xml:space="preserve">ratioNpc0</t>
@@ -736,7 +730,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -772,6 +766,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="3">
@@ -822,7 +822,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -849,6 +849,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1036,8 +1040,8 @@
   </sheetPr>
   <dimension ref="A1:R107"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I47" activeCellId="0" sqref="I47:J47"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E16" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H49" activeCellId="0" sqref="H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.16796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2070,19 +2074,19 @@
       <c r="G48" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="H48" s="1" t="s">
+      <c r="H48" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="I48" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="I48" s="1" t="s">
+      <c r="J48" s="1" t="s">
         <v>161</v>
-      </c>
-      <c r="J48" s="1" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>123</v>
@@ -2091,110 +2095,110 @@
         <v>124</v>
       </c>
       <c r="D49" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G49" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="G49" s="1" t="s">
-        <v>165</v>
-      </c>
       <c r="H49" s="1" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C50" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="D50" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="G50" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="D50" s="5" t="s">
+      <c r="H50" s="4" t="s">
         <v>170</v>
-      </c>
-      <c r="G50" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="H50" s="4" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="G51" s="3" t="s">
         <v>173</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="G51" s="3" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="61.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="G52" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="B52" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D52" s="5" t="s">
+      <c r="H52" s="4" t="s">
         <v>177</v>
-      </c>
-      <c r="G52" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="H52" s="4" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D53" s="5" t="s">
         <v>136</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I53" s="4" t="s">
         <v>139</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G54" s="3" t="s">
         <v>143</v>
@@ -2202,16 +2206,16 @@
     </row>
     <row r="55" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G55" s="3" t="s">
         <v>130</v>
@@ -2219,76 +2223,76 @@
     </row>
     <row r="56" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="G56" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D56" s="5" t="s">
+      <c r="H56" s="4" t="s">
         <v>189</v>
-      </c>
-      <c r="G56" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="H56" s="4" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="H57" s="4" t="s">
         <v>192</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="G57" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="H57" s="4" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="C58" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="D58" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="C58" s="4" t="s">
+      <c r="G58" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="D58" s="5" t="s">
+      <c r="H58" s="4" t="s">
         <v>198</v>
-      </c>
-      <c r="G58" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="H58" s="4" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G59" s="3" t="s">
         <v>130</v>
@@ -2296,62 +2300,62 @@
     </row>
     <row r="60" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="G60" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="D60" s="5" t="s">
+      <c r="H60" s="4" t="s">
         <v>204</v>
-      </c>
-      <c r="G60" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="H60" s="4" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D61" s="5" t="s">
         <v>136</v>
       </c>
       <c r="G61" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="H61" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="I61" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="H61" s="4" t="s">
+      <c r="J61" s="4" t="s">
         <v>209</v>
-      </c>
-      <c r="I61" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="J61" s="4" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G62" s="4" t="s">
         <v>143</v>
@@ -2359,88 +2363,88 @@
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="G63" s="4" t="s">
         <v>126</v>
       </c>
       <c r="I63" s="4" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D64" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="B64" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C64" s="1" t="s">
+      <c r="G64" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="D64" s="5" t="s">
+      <c r="I64" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="G64" s="4" t="s">
+      <c r="J64" s="4" t="s">
         <v>220</v>
-      </c>
-      <c r="I64" s="4" t="s">
-        <v>221</v>
-      </c>
-      <c r="J64" s="4" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>223</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>225</v>
       </c>
       <c r="G65" s="1" t="s">
         <v>130</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G66" s="1" t="s">
         <v>130</v>
       </c>
       <c r="H66" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added check to see if there is enough glass in the window.
</commit_message>
<xml_diff>
--- a/npc/npc.xlsx
+++ b/npc/npc.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="229">
   <si>
     <t xml:space="preserve">Scene</t>
   </si>
@@ -520,6 +520,12 @@
   </si>
   <si>
     <t xml:space="preserve">Graduate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scaleNpc11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brrrrr I can feel the breeze already, make sure the window is full of glass.</t>
   </si>
   <si>
     <t xml:space="preserve">ratioNpc0</t>
@@ -730,7 +736,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -766,12 +772,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="3">
@@ -822,7 +822,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -849,10 +849,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1040,8 +1036,8 @@
   </sheetPr>
   <dimension ref="A1:R107"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E16" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H49" activeCellId="0" sqref="H49"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A32" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G50" activeCellId="0" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.16796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2074,7 +2070,7 @@
       <c r="G48" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="H48" s="7" t="s">
+      <c r="H48" s="4" t="s">
         <v>147</v>
       </c>
       <c r="I48" s="1" t="s">
@@ -2105,103 +2101,116 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1" t="s">
+      <c r="A50" s="0" t="s">
         <v>165</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="D50" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="G50" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="H50" s="4" t="s">
-        <v>170</v>
-      </c>
+      <c r="E50" s="0"/>
+      <c r="F50" s="0"/>
+      <c r="G50" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="H50" s="0"/>
+      <c r="I50" s="0"/>
+      <c r="J50" s="0"/>
+      <c r="K50" s="0"/>
+      <c r="L50" s="0"/>
+      <c r="M50" s="0"/>
+      <c r="N50" s="0"/>
+      <c r="O50" s="0"/>
+      <c r="P50" s="0"/>
+      <c r="Q50" s="0"/>
+      <c r="R50" s="0"/>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="G51" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="D51" s="1" t="s">
+      <c r="H51" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="G51" s="3" t="s">
+    </row>
+    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="52" customFormat="false" ht="61.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="1" t="s">
+      <c r="B52" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="B52" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="D52" s="5" t="s">
+      <c r="G52" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="G52" s="3" t="s">
+    </row>
+    <row r="53" customFormat="false" ht="61.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="H52" s="4" t="s">
+      <c r="B53" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D53" s="5" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="1" t="s">
+      <c r="G53" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="B53" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="G53" s="3" t="s">
+      <c r="H53" s="4" t="s">
         <v>179</v>
-      </c>
-      <c r="H53" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="I53" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="J53" s="4" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="H54" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="D54" s="5" t="s">
+      <c r="I54" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="J54" s="4" t="s">
         <v>183</v>
-      </c>
-      <c r="G54" s="3" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2209,16 +2218,16 @@
         <v>184</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D55" s="5" t="s">
         <v>185</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>130</v>
+        <v>143</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2226,76 +2235,76 @@
         <v>186</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D56" s="5" t="s">
         <v>187</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="H56" s="4" t="s">
-        <v>189</v>
+        <v>130</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="G57" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="B57" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="D57" s="5" t="s">
+      <c r="H57" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="G57" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="H57" s="4" t="s">
+    </row>
+    <row r="58" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="58" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="6" t="s">
+      <c r="B58" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D58" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="G58" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="H58" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="C58" s="4" t="s">
+    </row>
+    <row r="59" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="D58" s="5" t="s">
+      <c r="B59" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="G58" s="3" t="s">
+      <c r="C59" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="H58" s="4" t="s">
+      <c r="D59" s="5" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="59" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="1" t="s">
+      <c r="G59" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="B59" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="D59" s="6" t="s">
+      <c r="H59" s="4" t="s">
         <v>200</v>
-      </c>
-      <c r="G59" s="3" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2303,62 +2312,62 @@
         <v>201</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="D60" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="D60" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="G60" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="H60" s="4" t="s">
-        <v>204</v>
+      <c r="G60" s="3" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="G61" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="B61" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="G61" s="4" t="s">
+      <c r="H61" s="4" t="s">
         <v>206</v>
-      </c>
-      <c r="H61" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="I61" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="J61" s="4" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="G62" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="H62" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="I62" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="B62" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="D62" s="5" t="s">
+      <c r="J62" s="4" t="s">
         <v>211</v>
-      </c>
-      <c r="G62" s="4" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2366,92 +2375,106 @@
         <v>212</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="D63" s="5" t="s">
         <v>213</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="I63" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="J63" s="4" t="s">
-        <v>209</v>
+        <v>143</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D64" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="B64" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="C64" s="1" t="s">
+      <c r="G64" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="I64" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="D64" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="G64" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="I64" s="4" t="s">
-        <v>219</v>
-      </c>
       <c r="J64" s="4" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="G65" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="I65" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="B65" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="C65" s="1" t="s">
+      <c r="J65" s="4" t="s">
         <v>222</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="G65" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="H65" s="1" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D66" s="1" t="s">
         <v>225</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>226</v>
       </c>
       <c r="G66" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="H66" s="4" t="s">
+      <c r="H66" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C67" s="1" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D67" s="5"/>
+      <c r="D67" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H67" s="4" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="68" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D68" s="6"/>
+      <c r="D68" s="5"/>
     </row>
     <row r="69" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D69" s="6"/>

</xml_diff>

<commit_message>
Pushed Isaacs fix and window 4 now works
</commit_message>
<xml_diff>
--- a/npc/npc.xlsx
+++ b/npc/npc.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="231">
   <si>
     <t xml:space="preserve">Scene</t>
   </si>
@@ -526,6 +526,16 @@
   </si>
   <si>
     <t xml:space="preserve">Brrrrr I can feel the breeze already, make sure the window is full of glass.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scaleNpc12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We’re working in blocks here, that scale factor isn’t a whole number. 
+Try again but make it a whole number.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On it!</t>
   </si>
   <si>
     <t xml:space="preserve">ratioNpc0</t>
@@ -604,9 +614,6 @@
   <si>
     <t xml:space="preserve">Before we start I need you to make me a .... I mean teach you about ratios, by making me chocolate milk. 
 Put 2 parts Cocoa beans to 1 part Milk into the cauldron and tap it with your wand.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">On it!</t>
   </si>
   <si>
     <t xml:space="preserve">scriptevent ratio:npc 3</t>
@@ -1036,8 +1043,8 @@
   </sheetPr>
   <dimension ref="A1:R107"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A32" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G50" activeCellId="0" sqref="G50"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E34" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H51" activeCellId="0" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.16796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2101,104 +2108,88 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
+      <c r="A50" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B50" s="0" t="s">
+      <c r="B50" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C50" s="0" t="s">
+      <c r="C50" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="D50" s="0" t="s">
+      <c r="D50" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="E50" s="0"/>
-      <c r="F50" s="0"/>
-      <c r="G50" s="0" t="s">
+      <c r="G50" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="H50" s="0"/>
-      <c r="I50" s="0"/>
-      <c r="J50" s="0"/>
-      <c r="K50" s="0"/>
-      <c r="L50" s="0"/>
-      <c r="M50" s="0"/>
-      <c r="N50" s="0"/>
-      <c r="O50" s="0"/>
-      <c r="P50" s="0"/>
-      <c r="Q50" s="0"/>
-      <c r="R50" s="0"/>
-    </row>
-    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="51" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
         <v>167</v>
       </c>
       <c r="B51" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D51" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="G51" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="G51" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="H51" s="4" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D52" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="B52" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D52" s="1" t="s">
+      <c r="G52" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="G52" s="3" t="s">
+      <c r="H52" s="4" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="61.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
         <v>176</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D53" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>177</v>
       </c>
       <c r="G53" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="H53" s="4" t="s">
-        <v>179</v>
-      </c>
     </row>
     <row r="54" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D54" s="5" t="s">
         <v>180</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>136</v>
       </c>
       <c r="G54" s="3" t="s">
         <v>181</v>
@@ -2206,122 +2197,125 @@
       <c r="H54" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="I54" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="J54" s="4" t="s">
-        <v>183</v>
-      </c>
     </row>
     <row r="55" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="G55" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="B55" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D55" s="5" t="s">
+      <c r="H55" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="G55" s="3" t="s">
-        <v>143</v>
+      <c r="I55" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="J55" s="4" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>130</v>
+        <v>143</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="H57" s="4" t="s">
-        <v>191</v>
+        <v>130</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D58" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="B58" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C58" s="1" t="s">
+      <c r="G58" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="D58" s="5" t="s">
+      <c r="H58" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="G58" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="H58" s="4" t="s">
+    </row>
+    <row r="59" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="59" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="6" t="s">
+      <c r="B59" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D59" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="G59" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="H59" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="C59" s="4" t="s">
+    </row>
+    <row r="60" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="D59" s="5" t="s">
+      <c r="B60" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="G59" s="3" t="s">
+      <c r="C60" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="H59" s="4" t="s">
+      <c r="D60" s="5" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="60" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="1" t="s">
+      <c r="G60" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="D60" s="6" t="s">
+      <c r="H60" s="4" t="s">
         <v>202</v>
-      </c>
-      <c r="G60" s="3" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2329,62 +2323,62 @@
         <v>203</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="D61" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="D61" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="G61" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="H61" s="4" t="s">
-        <v>206</v>
+      <c r="G61" s="3" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="G62" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="B62" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="D62" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="G62" s="4" t="s">
+      <c r="H62" s="4" t="s">
         <v>208</v>
-      </c>
-      <c r="H62" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="I62" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="J62" s="4" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="G63" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="H63" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="I63" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="B63" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="D63" s="5" t="s">
+      <c r="J63" s="4" t="s">
         <v>213</v>
-      </c>
-      <c r="G63" s="4" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2392,92 +2386,106 @@
         <v>214</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="D64" s="5" t="s">
         <v>215</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="I64" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="J64" s="4" t="s">
-        <v>211</v>
+        <v>143</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D65" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="B65" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C65" s="1" t="s">
+      <c r="G65" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="I65" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="D65" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="G65" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="I65" s="4" t="s">
-        <v>221</v>
-      </c>
       <c r="J65" s="4" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="G66" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="I66" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="B66" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="C66" s="1" t="s">
+      <c r="J66" s="4" t="s">
         <v>224</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="G66" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="H66" s="1" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="D67" s="1" t="s">
         <v>227</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>228</v>
       </c>
       <c r="G67" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="H67" s="4" t="s">
+      <c r="H67" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A68" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C68" s="1" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="68" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D68" s="5"/>
+      <c r="D68" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H68" s="4" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="69" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D69" s="6"/>
+      <c r="D69" s="5"/>
     </row>
     <row r="70" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D70" s="6"/>

</xml_diff>